<commit_message>
SRS and Test Cases Updated
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="212">
   <si>
     <t>Fail</t>
   </si>
@@ -160,22 +160,6 @@
     <t>user is registered successfully. The minimum length is 1 character</t>
   </si>
   <si>
-    <t>Register with name longer than 30 characters</t>
-  </si>
-  <si>
-    <t>1: Open blog "Register" page
-2: Type "test{today's date}@test.com" in "Email" field
-3: Type "Ivan Ivanov Ivan Ivanov Ivan Iv" in "Full Name" field
-4: Type "123456" in "Password" field
-5: Type "123456"in "Confirm Password"field 6: Click on "Register" button</t>
-  </si>
-  <si>
-    <t>"The field Full Name must be a string with a maximum length of 30." message should be shown to user</t>
-  </si>
-  <si>
-    <t>user is registered successfully. The maximum length is 50 characters</t>
-  </si>
-  <si>
     <t>1: Open blog "Register" page
 2: Type "test{today's date}@test.com" in "Email" field
 3: Type "1van Ivanov" in "Full Name" field
@@ -221,23 +205,7 @@
 5: Type "12345"in "Confirm Password"field 6: Click on "Register" button</t>
   </si>
   <si>
-    <t>Register with password longer than 30 characters</t>
-  </si>
-  <si>
-    <t>1: Open blog "Register" page
-2: Type "test{today's date}@test.com" in "Email" field
-3: Type "Ivan Ivanov" in "Full Name" field
-4: Type "0123456789012345678901234567891" in "Password" field
-5: Type "0123456789012345678901234567891" in "Confirm Password"field 6: Click on "Register" button</t>
-  </si>
-  <si>
     <t>"Password must be at least 6 symbols" message should be shown to user</t>
-  </si>
-  <si>
-    <t>"Password must maximum 30 symbols long." message should be shown to user</t>
-  </si>
-  <si>
-    <t>user is registered successfully. The maximum length is 100 characters, after that "The Password must be at least 1 characters long." message is shown to user</t>
   </si>
   <si>
     <t>Register with empty "Password" field</t>
@@ -759,9 +727,6 @@
     <t>RP_TC15</t>
   </si>
   <si>
-    <t>RP_TC16</t>
-  </si>
-  <si>
     <t>LP_TC1</t>
   </si>
   <si>
@@ -847,6 +812,32 @@
   </si>
   <si>
     <t>5. Tests on  "Edit Users" page</t>
+  </si>
+  <si>
+    <t>Register with name longer than 50 characters</t>
+  </si>
+  <si>
+    <t>"The field Full Name must be a string with a maximum length of 50." message should be shown to user</t>
+  </si>
+  <si>
+    <t>Register with password longer than 50 characters</t>
+  </si>
+  <si>
+    <t>"Password must maximum 50 symbols long." message should be shown to user</t>
+  </si>
+  <si>
+    <t>1: Open blog "Register" page
+2: Type "test{today's date}@test.com" in "Email" field
+3: Type any name with more that 50 characters in "Full Name" field
+4: Type "123456" in "Password" field
+5: Type "123456"in "Confirm Password"field 6: Click on "Register" button</t>
+  </si>
+  <si>
+    <t>1: Open blog "Register" page
+2: Type "test{today's date}@test.com" in "Email" field
+3: Type "Ivan Ivanov" in "Full Name" field
+4: Type any password longer than 50 symbols in "Password" field
+5: Type "0123456789012345678901234567891" in "Confirm Password"field 6: Click on "Register" button</t>
   </si>
 </sst>
 </file>
@@ -1297,7 +1288,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1395,9 +1386,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1419,11 +1407,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1434,23 +1422,38 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1482,9 +1485,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1497,29 +1497,17 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4124,10 +4112,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R544"/>
+  <dimension ref="A1:R543"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4148,95 +4136,95 @@
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="45"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="44"/>
       <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="45"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="44"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="70" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
+      <c r="B3" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="12.75">
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="1:15" s="23" customFormat="1" ht="12.75">
+    <row r="5" spans="1:15" s="23" customFormat="1" ht="25.5">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4244,7 +4232,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="33">
-        <f>COUNTIF(J12:J128,"Pass")</f>
+        <f>COUNTIF(J12:J127,"Pass")</f>
         <v>29</v>
       </c>
       <c r="C6" s="33"/>
@@ -4252,18 +4240,18 @@
         <v>14</v>
       </c>
       <c r="E6" s="10">
-        <f>COUNTIF(J10:J751,"Pending")</f>
+        <f>COUNTIF(J10:J750,"Pending")</f>
         <v>0</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4271,153 +4259,153 @@
         <v>0</v>
       </c>
       <c r="B7" s="34">
-        <f>COUNTIF(J12:J128,"Fail")</f>
-        <v>15</v>
+        <f>COUNTIF(J12:J127,"Fail")</f>
+        <v>14</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF(A12:A128,"TC*")</f>
+        <f>COUNTIF(A12:A127,"TC*")</f>
         <v>0</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="52" t="s">
+      <c r="C9" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="80" t="s">
+      <c r="E9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="76" t="s">
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="72" t="s">
+      <c r="J9" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="51" t="s">
+      <c r="K9" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="M9" s="51" t="s">
+      <c r="L9" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M9" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="72" t="s">
+      <c r="N9" s="57" t="s">
         <v>10</v>
       </c>
       <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" s="19" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="72"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" s="26" customFormat="1" ht="15">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="79"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="81"/>
     </row>
     <row r="12" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A12" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="55"/>
+      <c r="A12" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="54"/>
     </row>
     <row r="13" spans="1:15" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A13" s="30" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
+        <v>58</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
       <c r="H13" s="28"/>
-      <c r="I13" s="47">
+      <c r="I13" s="46">
         <v>42841</v>
       </c>
       <c r="J13" s="29" t="s">
@@ -4425,7 +4413,7 @@
       </c>
       <c r="K13" s="29"/>
       <c r="L13" s="29" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>18</v>
@@ -4434,7 +4422,7 @@
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A14" s="30" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>19</v>
@@ -4443,13 +4431,13 @@
       <c r="D14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
       <c r="H14" s="28"/>
-      <c r="I14" s="47">
+      <c r="I14" s="46">
         <v>42841</v>
       </c>
       <c r="J14" s="29" t="s">
@@ -4457,7 +4445,7 @@
       </c>
       <c r="K14" s="29"/>
       <c r="L14" s="29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>18</v>
@@ -4466,22 +4454,22 @@
     </row>
     <row r="15" spans="1:15" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A15" s="30" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="28"/>
-      <c r="I15" s="47">
+      <c r="I15" s="46">
         <v>42841</v>
       </c>
       <c r="J15" s="29" t="s">
@@ -4491,7 +4479,7 @@
         <v>24</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M15" s="29" t="s">
         <v>18</v>
@@ -4500,22 +4488,22 @@
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A16" s="30" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="47">
+      <c r="I16" s="46">
         <v>42841</v>
       </c>
       <c r="J16" s="29" t="s">
@@ -4523,7 +4511,7 @@
       </c>
       <c r="K16" s="29"/>
       <c r="L16" s="29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M16" s="29" t="s">
         <v>18</v>
@@ -4532,7 +4520,7 @@
     </row>
     <row r="17" spans="1:18" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A17" s="30" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>27</v>
@@ -4541,13 +4529,13 @@
       <c r="D17" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="47">
+      <c r="I17" s="46">
         <v>42841</v>
       </c>
       <c r="J17" s="29" t="s">
@@ -4557,7 +4545,7 @@
         <v>30</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M17" s="29" t="s">
         <v>18</v>
@@ -4566,32 +4554,30 @@
     </row>
     <row r="18" spans="1:18" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A18" s="30" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>31</v>
+        <v>206</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
+        <v>210</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="47">
+      <c r="I18" s="46">
         <v>42841</v>
       </c>
       <c r="J18" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="29" t="s">
-        <v>34</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="K18" s="29"/>
       <c r="L18" s="29" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M18" s="29" t="s">
         <v>18</v>
@@ -4600,32 +4586,32 @@
     </row>
     <row r="19" spans="1:18" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A19" s="30" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="28"/>
-      <c r="I19" s="47">
+      <c r="I19" s="46">
         <v>42841</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M19" s="29" t="s">
         <v>18</v>
@@ -4634,22 +4620,22 @@
     </row>
     <row r="20" spans="1:18" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A20" s="30" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
+        <v>44</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="47">
+      <c r="I20" s="46">
         <v>42841</v>
       </c>
       <c r="J20" s="29" t="s">
@@ -4657,7 +4643,7 @@
       </c>
       <c r="K20" s="29"/>
       <c r="L20" s="29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M20" s="29" t="s">
         <v>18</v>
@@ -4666,22 +4652,22 @@
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A21" s="30" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
+        <v>38</v>
+      </c>
+      <c r="E21" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="47">
+      <c r="I21" s="46">
         <v>42841</v>
       </c>
       <c r="J21" s="29" t="s">
@@ -4689,135 +4675,135 @@
       </c>
       <c r="K21" s="29"/>
       <c r="L21" s="29" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M21" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N21" s="27"/>
     </row>
-    <row r="22" spans="1:18" s="31" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="22" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A22" s="30" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="40"/>
       <c r="D22" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="47">
+      <c r="I22" s="46">
         <v>42841</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43" t="s">
-        <v>168</v>
+        <v>0</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>161</v>
       </c>
       <c r="M22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N22" s="32"/>
     </row>
-    <row r="23" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="23" spans="1:18" s="31" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A23" s="30" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>44</v>
+        <v>208</v>
       </c>
       <c r="C23" s="40"/>
       <c r="D23" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
+        <v>211</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="47">
+      <c r="I23" s="46">
         <v>42841</v>
       </c>
       <c r="J23" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K23" s="29" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L23" s="29" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N23" s="32"/>
-    </row>
-    <row r="24" spans="1:18" s="31" customFormat="1" ht="153" outlineLevel="1">
+      <c r="N23" s="42"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+    </row>
+    <row r="24" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A24" s="30" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
+        <v>48</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="28"/>
-      <c r="I24" s="47">
+      <c r="I24" s="46">
         <v>42841</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="L24" s="29" t="s">
-        <v>169</v>
+        <v>13</v>
+      </c>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="M24" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N24" s="42"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
+      <c r="N24" s="32"/>
     </row>
     <row r="25" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A25" s="30" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
+        <v>49</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="47">
+      <c r="I25" s="46">
         <v>42841</v>
       </c>
       <c r="J25" s="29" t="s">
@@ -4825,31 +4811,31 @@
       </c>
       <c r="K25" s="38"/>
       <c r="L25" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M25" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N25" s="32"/>
     </row>
-    <row r="26" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="26" spans="1:18" s="31" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="30" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
+        <v>52</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="28"/>
-      <c r="I26" s="47">
+      <c r="I26" s="46">
         <v>42841</v>
       </c>
       <c r="J26" s="29" t="s">
@@ -4857,7 +4843,7 @@
       </c>
       <c r="K26" s="38"/>
       <c r="L26" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M26" s="29" t="s">
         <v>18</v>
@@ -4866,22 +4852,22 @@
     </row>
     <row r="27" spans="1:18" s="31" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A27" s="30" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
+        <v>55</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="47">
+      <c r="I27" s="46">
         <v>42841</v>
       </c>
       <c r="J27" s="29" t="s">
@@ -4889,83 +4875,83 @@
       </c>
       <c r="K27" s="38"/>
       <c r="L27" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M27" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N27" s="32"/>
     </row>
-    <row r="28" spans="1:18" s="31" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A28" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="47">
-        <v>42841</v>
-      </c>
-      <c r="J28" s="29" t="s">
+    <row r="28" spans="1:18" s="3" customFormat="1" ht="12.75">
+      <c r="A28" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="54"/>
+    </row>
+    <row r="29" spans="1:18" s="31" customFormat="1" ht="63.75" outlineLevel="1">
+      <c r="A29" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="46">
+        <v>42843</v>
+      </c>
+      <c r="J29" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="M28" s="29" t="s">
+      <c r="K29" s="38"/>
+      <c r="L29" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="M29" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N28" s="32"/>
-    </row>
-    <row r="29" spans="1:18" s="3" customFormat="1" ht="12.75">
-      <c r="A29" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="55"/>
+      <c r="N29" s="32"/>
     </row>
     <row r="30" spans="1:18" s="31" customFormat="1" ht="51" outlineLevel="1">
       <c r="A30" s="30" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>74</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C30" s="32"/>
       <c r="D30" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
+        <v>70</v>
+      </c>
+      <c r="E30" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="47">
+      <c r="I30" s="46">
         <v>42843</v>
       </c>
       <c r="J30" s="29" t="s">
@@ -4973,31 +4959,33 @@
       </c>
       <c r="K30" s="38"/>
       <c r="L30" s="38" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="M30" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N30" s="32"/>
     </row>
-    <row r="31" spans="1:18" s="31" customFormat="1" ht="51" outlineLevel="1">
+    <row r="31" spans="1:18" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A31" s="30" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="32"/>
+        <v>63</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>67</v>
+      </c>
       <c r="D31" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
+        <v>71</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="47">
+      <c r="I31" s="46">
         <v>42843</v>
       </c>
       <c r="J31" s="29" t="s">
@@ -5005,33 +4993,33 @@
       </c>
       <c r="K31" s="38"/>
       <c r="L31" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M31" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N31" s="32"/>
     </row>
-    <row r="32" spans="1:18" s="31" customFormat="1" ht="51" outlineLevel="1">
+    <row r="32" spans="1:18" s="31" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A32" s="30" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B32" s="40" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
+        <v>72</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="28"/>
-      <c r="I32" s="47">
+      <c r="I32" s="46">
         <v>42843</v>
       </c>
       <c r="J32" s="29" t="s">
@@ -5039,33 +5027,33 @@
       </c>
       <c r="K32" s="38"/>
       <c r="L32" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M32" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N32" s="32"/>
     </row>
-    <row r="33" spans="1:14" s="31" customFormat="1" ht="51" outlineLevel="1">
+    <row r="33" spans="1:14" s="31" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A33" s="30" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="56" t="s">
-        <v>153</v>
-      </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
+        <v>128</v>
+      </c>
+      <c r="E33" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="47">
+      <c r="I33" s="46">
         <v>42843</v>
       </c>
       <c r="J33" s="29" t="s">
@@ -5073,85 +5061,85 @@
       </c>
       <c r="K33" s="38"/>
       <c r="L33" s="38" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="M33" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N33" s="32"/>
     </row>
-    <row r="34" spans="1:14" s="31" customFormat="1" ht="25.5" outlineLevel="1">
-      <c r="A34" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B34" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="D34" s="29" t="s">
+    <row r="34" spans="1:14" s="3" customFormat="1" ht="12.75">
+      <c r="A34" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="54"/>
+    </row>
+    <row r="35" spans="1:14" s="31" customFormat="1" ht="140.25" outlineLevel="1">
+      <c r="A35" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="47">
+      <c r="E35" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="46">
         <v>42843</v>
       </c>
-      <c r="J34" s="29" t="s">
+      <c r="J35" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="38"/>
-      <c r="L34" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="M34" s="29" t="s">
+      <c r="K35" s="38"/>
+      <c r="L35" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="M35" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="N34" s="32"/>
-    </row>
-    <row r="35" spans="1:14" s="3" customFormat="1" ht="12.75">
-      <c r="A35" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="55"/>
-    </row>
-    <row r="36" spans="1:14" s="31" customFormat="1" ht="140.25" outlineLevel="1">
+      <c r="N35" s="32"/>
+    </row>
+    <row r="36" spans="1:14" s="31" customFormat="1" ht="51" outlineLevel="1">
       <c r="A36" s="30" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B36" s="40" t="s">
         <v>76</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
+        <v>77</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="47">
+      <c r="I36" s="46">
         <v>42843</v>
       </c>
       <c r="J36" s="29" t="s">
@@ -5159,33 +5147,33 @@
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="38" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M36" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N36" s="32"/>
     </row>
-    <row r="37" spans="1:14" s="31" customFormat="1" ht="51" outlineLevel="1">
+    <row r="37" spans="1:14" s="31" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A37" s="30" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
+        <v>80</v>
+      </c>
+      <c r="E37" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="47">
+      <c r="I37" s="46">
         <v>42843</v>
       </c>
       <c r="J37" s="29" t="s">
@@ -5193,7 +5181,7 @@
       </c>
       <c r="K37" s="38"/>
       <c r="L37" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M37" s="29" t="s">
         <v>18</v>
@@ -5202,102 +5190,104 @@
     </row>
     <row r="38" spans="1:14" s="31" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A38" s="30" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
+        <v>81</v>
+      </c>
+      <c r="E38" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="47">
+      <c r="I38" s="46">
         <v>42843</v>
       </c>
       <c r="J38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="38"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="47" t="s">
+        <v>151</v>
+      </c>
       <c r="L38" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M38" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N38" s="32"/>
     </row>
-    <row r="39" spans="1:14" s="31" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="39" spans="1:14" s="31" customFormat="1" ht="102" outlineLevel="1">
       <c r="A39" s="30" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
+        <v>137</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="47">
+      <c r="I39" s="46">
         <v>42843</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K39" s="48" t="s">
-        <v>159</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="K39" s="47"/>
       <c r="L39" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M39" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N39" s="32"/>
     </row>
-    <row r="40" spans="1:14" s="31" customFormat="1" ht="102" outlineLevel="1">
+    <row r="40" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A40" s="30" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
+        <v>82</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
       <c r="H40" s="28"/>
-      <c r="I40" s="47">
+      <c r="I40" s="46">
         <v>42843</v>
       </c>
       <c r="J40" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="48"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="47" t="s">
+        <v>151</v>
+      </c>
       <c r="L40" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M40" s="29" t="s">
         <v>18</v>
@@ -5306,122 +5296,122 @@
     </row>
     <row r="41" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A41" s="30" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
+        <v>86</v>
+      </c>
+      <c r="E41" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
       <c r="H41" s="28"/>
-      <c r="I41" s="47">
+      <c r="I41" s="46">
         <v>42843</v>
       </c>
       <c r="J41" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K41" s="48" t="s">
-        <v>159</v>
+      <c r="K41" s="47" t="s">
+        <v>148</v>
       </c>
       <c r="L41" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M41" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N41" s="32"/>
     </row>
-    <row r="42" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
-      <c r="A42" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="29" t="s">
+    <row r="42" spans="1:14" s="3" customFormat="1" ht="12.75">
+      <c r="A42" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="54"/>
+    </row>
+    <row r="43" spans="1:14" s="31" customFormat="1" ht="165.75" outlineLevel="1">
+      <c r="A43" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="46">
+        <v>42843</v>
+      </c>
+      <c r="J43" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="M43" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N43" s="32"/>
+    </row>
+    <row r="44" spans="1:14" s="31" customFormat="1" ht="153" outlineLevel="1">
+      <c r="A44" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" s="57"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="47">
+      <c r="D44" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="46">
         <v>42843</v>
       </c>
-      <c r="J42" s="29" t="s">
+      <c r="J44" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K42" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="L42" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="M42" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N42" s="32"/>
-    </row>
-    <row r="43" spans="1:14" s="3" customFormat="1" ht="12.75">
-      <c r="A43" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="55"/>
-    </row>
-    <row r="44" spans="1:14" s="31" customFormat="1" ht="165.75" outlineLevel="1">
-      <c r="A44" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="E44" s="56" t="s">
-        <v>157</v>
-      </c>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="47">
-        <v>42843</v>
-      </c>
-      <c r="J44" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="38"/>
+      <c r="K44" s="47" t="s">
+        <v>150</v>
+      </c>
       <c r="L44" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M44" s="29" t="s">
         <v>18</v>
@@ -5430,68 +5420,68 @@
     </row>
     <row r="45" spans="1:14" s="31" customFormat="1" ht="153" outlineLevel="1">
       <c r="A45" s="30" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E45" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
+        <v>144</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
       <c r="H45" s="28"/>
-      <c r="I45" s="47">
+      <c r="I45" s="46">
         <v>42843</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K45" s="48" t="s">
-        <v>158</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="K45" s="38"/>
       <c r="L45" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M45" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N45" s="32"/>
     </row>
-    <row r="46" spans="1:14" s="31" customFormat="1" ht="153" outlineLevel="1">
+    <row r="46" spans="1:14" s="31" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A46" s="30" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
+        <v>139</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
       <c r="H46" s="28"/>
-      <c r="I46" s="47">
+      <c r="I46" s="46">
         <v>42843</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K46" s="38"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="47" t="s">
+        <v>150</v>
+      </c>
       <c r="L46" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M46" s="29" t="s">
         <v>18</v>
@@ -5500,330 +5490,328 @@
     </row>
     <row r="47" spans="1:14" s="31" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A47" s="30" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
+        <v>140</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
       <c r="H47" s="28"/>
-      <c r="I47" s="47">
+      <c r="I47" s="46">
         <v>42843</v>
       </c>
       <c r="J47" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K47" s="48" t="s">
-        <v>158</v>
+      <c r="K47" s="47" t="s">
+        <v>148</v>
       </c>
       <c r="L47" s="38" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="M47" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N47" s="32"/>
     </row>
-    <row r="48" spans="1:14" s="31" customFormat="1" ht="114.75" outlineLevel="1">
+    <row r="48" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A48" s="30" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B48" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="32" t="s">
-        <v>116</v>
-      </c>
       <c r="D48" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
+        <v>153</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="28"/>
-      <c r="I48" s="47">
+      <c r="I48" s="46">
         <v>42843</v>
       </c>
       <c r="J48" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K48" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="L48" s="38" t="s">
-        <v>169</v>
+        <v>13</v>
+      </c>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47" t="s">
+        <v>161</v>
       </c>
       <c r="M48" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N48" s="32"/>
     </row>
-    <row r="49" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="49" spans="1:14" s="31" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A49" s="30" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B49" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E49" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="56" t="s">
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="46">
+        <v>42843</v>
+      </c>
+      <c r="J49" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K49" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" s="47" t="s">
         <v>160</v>
-      </c>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="47">
-        <v>42843</v>
-      </c>
-      <c r="J49" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48" t="s">
-        <v>169</v>
       </c>
       <c r="M49" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N49" s="32"/>
     </row>
-    <row r="50" spans="1:14" s="31" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="50" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A50" s="30" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E50" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
+        <v>95</v>
+      </c>
+      <c r="E50" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="28"/>
-      <c r="I50" s="47">
+      <c r="I50" s="46">
         <v>42843</v>
       </c>
       <c r="J50" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="K50" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="L50" s="48" t="s">
-        <v>168</v>
+      <c r="K50" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="L50" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="M50" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N50" s="32"/>
     </row>
-    <row r="51" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="51" spans="1:14" s="31" customFormat="1" ht="51" outlineLevel="1">
       <c r="A51" s="30" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B51" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
+      <c r="E51" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="28"/>
-      <c r="I51" s="47">
+      <c r="I51" s="46">
         <v>42843</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K51" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="L51" s="48" t="s">
-        <v>168</v>
+        <v>13</v>
+      </c>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47" t="s">
+        <v>161</v>
       </c>
       <c r="M51" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N51" s="32"/>
     </row>
-    <row r="52" spans="1:14" s="31" customFormat="1" ht="51" outlineLevel="1">
+    <row r="52" spans="1:14" s="31" customFormat="1" ht="153" outlineLevel="1">
       <c r="A52" s="30" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
+        <v>141</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
       <c r="H52" s="28"/>
-      <c r="I52" s="47">
+      <c r="I52" s="46">
         <v>42843</v>
       </c>
       <c r="J52" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48" t="s">
-        <v>169</v>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="M52" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N52" s="32"/>
     </row>
-    <row r="53" spans="1:14" s="31" customFormat="1" ht="153" outlineLevel="1">
+    <row r="53" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A53" s="30" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="E53" s="56" t="s">
-        <v>162</v>
-      </c>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
+        <v>155</v>
+      </c>
+      <c r="E53" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="28"/>
-      <c r="I53" s="47">
+      <c r="I53" s="46">
         <v>42843</v>
       </c>
       <c r="J53" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38" t="s">
-        <v>169</v>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47" t="s">
+        <v>161</v>
       </c>
       <c r="M53" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N53" s="32"/>
     </row>
-    <row r="54" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A54" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="B54" s="40" t="s">
+    <row r="54" spans="1:14" s="3" customFormat="1" ht="12.75">
+      <c r="A54" s="52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="53"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="53"/>
+      <c r="N54" s="54"/>
+    </row>
+    <row r="55" spans="1:14" s="31" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="A55" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="46">
+        <v>42847</v>
+      </c>
+      <c r="J55" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="M55" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="N55" s="32"/>
+    </row>
+    <row r="56" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
+      <c r="A56" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E54" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="47">
-        <v>42843</v>
-      </c>
-      <c r="J54" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="M54" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N54" s="32"/>
-    </row>
-    <row r="55" spans="1:14" s="3" customFormat="1" ht="12.75">
-      <c r="A55" s="53" t="s">
-        <v>214</v>
-      </c>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="54"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="54"/>
-      <c r="L55" s="54"/>
-      <c r="M55" s="54"/>
-      <c r="N55" s="55"/>
-    </row>
-    <row r="56" spans="1:14" s="31" customFormat="1" ht="25.5" outlineLevel="1">
-      <c r="A56" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="B56" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
+      <c r="E56" s="50" t="s">
+        <v>156</v>
+      </c>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="28"/>
-      <c r="I56" s="47">
+      <c r="I56" s="46">
         <v>42847</v>
       </c>
       <c r="J56" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48" t="s">
-        <v>168</v>
+      <c r="K56" s="47"/>
+      <c r="L56" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="M56" s="29" t="s">
         <v>18</v>
@@ -5832,66 +5820,68 @@
     </row>
     <row r="57" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A57" s="30" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="E57" s="56" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" s="57"/>
-      <c r="G57" s="57"/>
+        <v>157</v>
+      </c>
+      <c r="E57" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
       <c r="H57" s="28"/>
-      <c r="I57" s="47">
+      <c r="I57" s="46">
         <v>42847</v>
       </c>
       <c r="J57" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48" t="s">
-        <v>168</v>
+      <c r="K57" s="47"/>
+      <c r="L57" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="M57" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N57" s="32"/>
     </row>
-    <row r="58" spans="1:14" s="31" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="58" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A58" s="30" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C58" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E58" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="E58" s="56" t="s">
-        <v>166</v>
-      </c>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
       <c r="H58" s="28"/>
-      <c r="I58" s="47">
+      <c r="I58" s="46">
         <v>42847</v>
       </c>
       <c r="J58" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K58" s="48"/>
-      <c r="L58" s="48" t="s">
-        <v>168</v>
+        <v>0</v>
+      </c>
+      <c r="K58" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="L58" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="M58" s="29" t="s">
         <v>18</v>
@@ -5900,73 +5890,46 @@
     </row>
     <row r="59" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A59" s="30" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E59" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="F59" s="57"/>
-      <c r="G59" s="57"/>
+        <v>123</v>
+      </c>
+      <c r="E59" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
       <c r="H59" s="28"/>
-      <c r="I59" s="47">
+      <c r="I59" s="46">
         <v>42847</v>
       </c>
       <c r="J59" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K59" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="L59" s="48" t="s">
-        <v>168</v>
+        <v>13</v>
+      </c>
+      <c r="K59" s="47"/>
+      <c r="L59" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="M59" s="29" t="s">
         <v>18</v>
       </c>
       <c r="N59" s="32"/>
     </row>
-    <row r="60" spans="1:14" s="31" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A60" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="B60" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E60" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="28"/>
-      <c r="I60" s="47">
-        <v>42847</v>
-      </c>
-      <c r="J60" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="M60" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="N60" s="32"/>
+    <row r="60" spans="1:14" ht="12" customHeight="1">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
     </row>
     <row r="61" spans="1:14" ht="12" customHeight="1">
       <c r="B61"/>
@@ -6049,9 +6012,7 @@
       <c r="M69"/>
       <c r="N69"/>
     </row>
-    <row r="70" spans="2:14" ht="12" customHeight="1">
-      <c r="B70"/>
-      <c r="C70"/>
+    <row r="70" spans="2:14" ht="13.5">
       <c r="J70"/>
       <c r="K70"/>
       <c r="L70"/>
@@ -9369,53 +9330,23 @@
       <c r="M543"/>
       <c r="N543"/>
     </row>
-    <row r="544" spans="10:14" ht="13.5">
-      <c r="J544"/>
-      <c r="K544"/>
-      <c r="L544"/>
-      <c r="M544"/>
-      <c r="N544"/>
-    </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="A55:N55"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="A43:N43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="A35:N35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:H10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E15:G15"/>
+  <mergeCells count="69">
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A28:N28"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B1:E2"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -9432,22 +9363,44 @@
     <mergeCell ref="A11:N11"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="A29:N29"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A34:N34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A42:N42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="A54:N54"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding the other tests from Registration page - they failed because of the blog
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="213">
   <si>
     <t>Fail</t>
   </si>
@@ -838,6 +838,9 @@
 3: Type "Ivan Ivanov" in "Full Name" field
 4: Type any password longer than 50 symbols in "Password" field
 5: Type "0123456789012345678901234567891" in "Confirm Password"field 6: Click on "Register" button</t>
+  </si>
+  <si>
+    <t>Iliya Iliev</t>
   </si>
 </sst>
 </file>
@@ -1407,11 +1410,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1422,23 +1425,38 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1470,9 +1488,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1485,29 +1500,17 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4114,8 +4117,8 @@
   </sheetPr>
   <dimension ref="A1:R543"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -4126,7 +4129,7 @@
     <col min="4" max="4" width="42.109375" customWidth="1"/>
     <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="39"/>
     <col min="11" max="13" width="13.109375" style="39" customWidth="1"/>
     <col min="14" max="14" width="18" style="37" customWidth="1"/>
@@ -4136,10 +4139,10 @@
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -4153,10 +4156,10 @@
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -4172,59 +4175,59 @@
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="26.4">
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
       <c r="O4" s="7"/>
     </row>
     <row r="5" spans="1:15" s="23" customFormat="1" ht="26.4">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4246,12 +4249,12 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4273,20 +4276,20 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
       <c r="O7" s="7"/>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -4299,76 +4302,76 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="E9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="75" t="s">
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="71" t="s">
+      <c r="J9" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="55" t="s">
         <v>16</v>
       </c>
       <c r="L9" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M9" s="50" t="s">
+      <c r="M9" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="71" t="s">
+      <c r="N9" s="57" t="s">
         <v>10</v>
       </c>
       <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" s="19" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="51"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="56"/>
       <c r="L10" s="49"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="71"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" s="26" customFormat="1" ht="15">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="78"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="81"/>
     </row>
     <row r="12" spans="1:15" s="3" customFormat="1" ht="13.2">
       <c r="A12" s="52" t="s">
@@ -4399,11 +4402,11 @@
       <c r="D13" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
       <c r="H13" s="28"/>
       <c r="I13" s="46">
         <v>42841</v>
@@ -4431,11 +4434,11 @@
       <c r="D14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
       <c r="H14" s="28"/>
       <c r="I14" s="46">
         <v>42841</v>
@@ -4463,14 +4466,14 @@
       <c r="D15" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="28"/>
       <c r="I15" s="46">
-        <v>42841</v>
+        <v>42869</v>
       </c>
       <c r="J15" s="29" t="s">
         <v>0</v>
@@ -4482,7 +4485,7 @@
         <v>160</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="N15" s="27"/>
     </row>
@@ -4497,11 +4500,11 @@
       <c r="D16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="28"/>
       <c r="I16" s="46">
         <v>42841</v>
@@ -4529,14 +4532,14 @@
       <c r="D17" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="28"/>
       <c r="I17" s="46">
-        <v>42841</v>
+        <v>42869</v>
       </c>
       <c r="J17" s="29" t="s">
         <v>0</v>
@@ -4548,7 +4551,7 @@
         <v>161</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="N17" s="27"/>
     </row>
@@ -4563,11 +4566,11 @@
       <c r="D18" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="28"/>
       <c r="I18" s="46">
         <v>42841</v>
@@ -4595,14 +4598,14 @@
       <c r="D19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="28"/>
       <c r="I19" s="46">
-        <v>42841</v>
+        <v>42869</v>
       </c>
       <c r="J19" s="29" t="s">
         <v>0</v>
@@ -4614,7 +4617,7 @@
         <v>161</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="N19" s="27"/>
     </row>
@@ -4629,11 +4632,11 @@
       <c r="D20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="28"/>
       <c r="I20" s="46">
         <v>42841</v>
@@ -4661,11 +4664,11 @@
       <c r="D21" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
       <c r="H21" s="28"/>
       <c r="I21" s="46">
         <v>42841</v>
@@ -4693,14 +4696,14 @@
       <c r="D22" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
       <c r="H22" s="28"/>
       <c r="I22" s="46">
-        <v>42841</v>
+        <v>42869</v>
       </c>
       <c r="J22" s="29" t="s">
         <v>0</v>
@@ -4712,7 +4715,7 @@
         <v>161</v>
       </c>
       <c r="M22" s="29" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="N22" s="32"/>
     </row>
@@ -4727,11 +4730,11 @@
       <c r="D23" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="28"/>
       <c r="I23" s="46">
         <v>42841</v>
@@ -4765,11 +4768,11 @@
       <c r="D24" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="28"/>
       <c r="I24" s="46">
         <v>42841</v>
@@ -4797,11 +4800,11 @@
       <c r="D25" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="28"/>
       <c r="I25" s="46">
         <v>42841</v>
@@ -4829,11 +4832,11 @@
       <c r="D26" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
       <c r="H26" s="28"/>
       <c r="I26" s="46">
         <v>42841</v>
@@ -4861,11 +4864,11 @@
       <c r="D27" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="28"/>
       <c r="I27" s="46">
         <v>42841</v>
@@ -4913,11 +4916,11 @@
       <c r="D29" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="28"/>
       <c r="I29" s="46">
         <v>42843</v>
@@ -4945,11 +4948,11 @@
       <c r="D30" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="28"/>
       <c r="I30" s="46">
         <v>42843</v>
@@ -4979,11 +4982,11 @@
       <c r="D31" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="28"/>
       <c r="I31" s="46">
         <v>42843</v>
@@ -5013,11 +5016,11 @@
       <c r="D32" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="28"/>
       <c r="I32" s="46">
         <v>42843</v>
@@ -5047,11 +5050,11 @@
       <c r="D33" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
       <c r="H33" s="28"/>
       <c r="I33" s="46">
         <v>42843</v>
@@ -5099,11 +5102,11 @@
       <c r="D35" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
       <c r="H35" s="28"/>
       <c r="I35" s="46">
         <v>42843</v>
@@ -5133,11 +5136,11 @@
       <c r="D36" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="28"/>
       <c r="I36" s="46">
         <v>42843</v>
@@ -5167,11 +5170,11 @@
       <c r="D37" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="55" t="s">
+      <c r="E37" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
       <c r="H37" s="28"/>
       <c r="I37" s="46">
         <v>42843</v>
@@ -5201,11 +5204,11 @@
       <c r="D38" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="55" t="s">
+      <c r="E38" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
       <c r="H38" s="28"/>
       <c r="I38" s="46">
         <v>42843</v>
@@ -5237,11 +5240,11 @@
       <c r="D39" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="55" t="s">
+      <c r="E39" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
       <c r="H39" s="28"/>
       <c r="I39" s="46">
         <v>42843</v>
@@ -5271,11 +5274,11 @@
       <c r="D40" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="55" t="s">
+      <c r="E40" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
       <c r="H40" s="28"/>
       <c r="I40" s="46">
         <v>42843</v>
@@ -5307,11 +5310,11 @@
       <c r="D41" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="55" t="s">
+      <c r="E41" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
       <c r="H41" s="28"/>
       <c r="I41" s="46">
         <v>42843</v>
@@ -5361,11 +5364,11 @@
       <c r="D43" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="E43" s="55" t="s">
+      <c r="E43" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
       <c r="H43" s="28"/>
       <c r="I43" s="46">
         <v>42843</v>
@@ -5395,11 +5398,11 @@
       <c r="D44" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
       <c r="H44" s="28"/>
       <c r="I44" s="46">
         <v>42843</v>
@@ -5431,11 +5434,11 @@
       <c r="D45" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
       <c r="H45" s="28"/>
       <c r="I45" s="46">
         <v>42843</v>
@@ -5465,11 +5468,11 @@
       <c r="D46" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="55" t="s">
+      <c r="E46" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
       <c r="H46" s="28"/>
       <c r="I46" s="46">
         <v>42843</v>
@@ -5501,11 +5504,11 @@
       <c r="D47" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="E47" s="55" t="s">
+      <c r="E47" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
       <c r="H47" s="28"/>
       <c r="I47" s="46">
         <v>42843</v>
@@ -5537,11 +5540,11 @@
       <c r="D48" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E48" s="55" t="s">
+      <c r="E48" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
       <c r="H48" s="28"/>
       <c r="I48" s="46">
         <v>42843</v>
@@ -5571,11 +5574,11 @@
       <c r="D49" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="55" t="s">
+      <c r="E49" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
       <c r="H49" s="28"/>
       <c r="I49" s="46">
         <v>42843</v>
@@ -5607,11 +5610,11 @@
       <c r="D50" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="E50" s="55" t="s">
+      <c r="E50" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
       <c r="H50" s="28"/>
       <c r="I50" s="46">
         <v>42843</v>
@@ -5643,11 +5646,11 @@
       <c r="D51" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="E51" s="55" t="s">
+      <c r="E51" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="28"/>
       <c r="I51" s="46">
         <v>42843</v>
@@ -5677,11 +5680,11 @@
       <c r="D52" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="55" t="s">
+      <c r="E52" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
       <c r="H52" s="28"/>
       <c r="I52" s="46">
         <v>42843</v>
@@ -5711,11 +5714,11 @@
       <c r="D53" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="55" t="s">
+      <c r="E53" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
       <c r="H53" s="28"/>
       <c r="I53" s="46">
         <v>42843</v>
@@ -5763,11 +5766,11 @@
       <c r="D55" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E55" s="55" t="s">
+      <c r="E55" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
       <c r="H55" s="28"/>
       <c r="I55" s="46">
         <v>42847</v>
@@ -5797,11 +5800,11 @@
       <c r="D56" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E56" s="55" t="s">
+      <c r="E56" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
       <c r="H56" s="28"/>
       <c r="I56" s="46">
         <v>42847</v>
@@ -5831,11 +5834,11 @@
       <c r="D57" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="E57" s="55" t="s">
+      <c r="E57" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
       <c r="H57" s="28"/>
       <c r="I57" s="46">
         <v>42847</v>
@@ -5865,11 +5868,11 @@
       <c r="D58" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E58" s="55" t="s">
+      <c r="E58" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
       <c r="H58" s="28"/>
       <c r="I58" s="46">
         <v>42847</v>
@@ -5901,11 +5904,11 @@
       <c r="D59" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E59" s="55" t="s">
+      <c r="E59" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
       <c r="H59" s="28"/>
       <c r="I59" s="46">
         <v>42847</v>
@@ -9332,44 +9335,21 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="A54:N54"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="A42:N42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="A34:N34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:H10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A28:N28"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B1:E2"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -9386,21 +9366,44 @@
     <mergeCell ref="A11:N11"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="A28:N28"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="A34:N34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="A42:N42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="A54:N54"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added more test cases for Login
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goychevl\Downloads\QA Automation SoftUni\TeamProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftUni\Team Papaya\QA-Automation-Team-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="258">
   <si>
     <t>Fail</t>
   </si>
@@ -982,12 +982,6 @@
   <si>
     <t>"The Full Name field is required."
 "The Password field is required." messages should be shown to user</t>
-  </si>
-  <si>
-    <t>RP_TC19</t>
-  </si>
-  <si>
-    <t>Register with empty e-mail three times</t>
   </si>
   <si>
     <t>Author</t>
@@ -1579,53 +1573,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1645,6 +1609,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1656,6 +1629,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1669,6 +1645,24 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1678,25 +1672,25 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4297,12 +4291,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T554"/>
+  <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="K16" sqref="K16"/>
+      <selection pane="topRight" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4325,10 +4319,10 @@
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -4350,15 +4344,15 @@
         <v>234</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -4377,84 +4371,84 @@
         <v>0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="82"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="2" t="s">
         <v>161</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="25.5">
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="79"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
       <c r="P4" s="7"/>
       <c r="T4" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="23" customFormat="1" ht="25.5">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="78"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
       <c r="P5" s="22"/>
       <c r="T5" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4462,27 +4456,27 @@
         <v>13</v>
       </c>
       <c r="B6" s="32">
-        <f>COUNTIF(I17:I138,"Pass")</f>
-        <v>35</v>
+        <f>COUNTIF(I17:I137,"Pass")</f>
+        <v>34</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="10">
-        <f>COUNTIF(I10:I761,"Pending")</f>
+        <f>COUNTIF(I10:I760,"Pending")</f>
         <v>0</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4490,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="33">
-        <f>COUNTIF(I17:I138,"Fail")</f>
+        <f>COUNTIF(I17:I137,"Fail")</f>
         <v>14</v>
       </c>
       <c r="C7" s="33"/>
@@ -4498,27 +4492,27 @@
         <v>6</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF(A17:A138,"TC*")</f>
+        <f>COUNTIF(A17:A137,"TC*")</f>
         <v>0</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -4532,102 +4526,102 @@
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="86" t="s">
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="57" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="62" t="s">
+      <c r="M9" s="57" t="s">
         <v>235</v>
       </c>
-      <c r="N9" s="62" t="s">
-        <v>253</v>
-      </c>
-      <c r="O9" s="64" t="s">
+      <c r="N9" s="57" t="s">
+        <v>251</v>
+      </c>
+      <c r="O9" s="76" t="s">
         <v>10</v>
       </c>
       <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:20" s="19" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="63"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="58"/>
       <c r="K10" s="48"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="64"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="76"/>
       <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:20" s="26" customFormat="1" ht="15">
-      <c r="A11" s="71"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="72"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="85"/>
+      <c r="O11" s="86"/>
     </row>
     <row r="12" spans="1:20" s="3" customFormat="1" ht="12.75">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="61"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="70"/>
+      <c r="M12" s="70"/>
+      <c r="N12" s="70"/>
+      <c r="O12" s="71"/>
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="76.5" customHeight="1" outlineLevel="1">
       <c r="A13" s="29" t="s">
@@ -4640,11 +4634,11 @@
       <c r="D13" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
       <c r="H13" s="45">
         <v>42841</v>
       </c>
@@ -4656,13 +4650,13 @@
         <v>159</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M13" s="50" t="s">
         <v>234</v>
       </c>
       <c r="N13" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O13" s="27"/>
     </row>
@@ -4677,11 +4671,11 @@
       <c r="D14" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
       <c r="H14" s="45">
         <v>42841</v>
       </c>
@@ -4697,7 +4691,7 @@
         <v>234</v>
       </c>
       <c r="N14" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O14" s="27"/>
     </row>
@@ -4712,11 +4706,11 @@
       <c r="D15" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="E15" s="69" t="s">
+      <c r="E15" s="61" t="s">
         <v>227</v>
       </c>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
       <c r="H15" s="45">
         <v>42841</v>
       </c>
@@ -4732,7 +4726,7 @@
         <v>234</v>
       </c>
       <c r="N15" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O15" s="27"/>
     </row>
@@ -4747,11 +4741,11 @@
       <c r="D16" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="61" t="s">
         <v>230</v>
       </c>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="45">
         <v>42841</v>
       </c>
@@ -4767,28 +4761,28 @@
         <v>234</v>
       </c>
       <c r="N16" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:19" s="3" customFormat="1" ht="12.75">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="61"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="71"/>
     </row>
     <row r="18" spans="1:19" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A18" s="29" t="s">
@@ -4801,11 +4795,11 @@
       <c r="D18" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="61" t="s">
         <v>238</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
       <c r="H18" s="45">
         <v>42841</v>
       </c>
@@ -4823,7 +4817,7 @@
         <v>234</v>
       </c>
       <c r="N18" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O18" s="27"/>
     </row>
@@ -4838,11 +4832,11 @@
       <c r="D19" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="45">
         <v>42841</v>
       </c>
@@ -4860,7 +4854,7 @@
         <v>234</v>
       </c>
       <c r="N19" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O19" s="27"/>
     </row>
@@ -4875,11 +4869,11 @@
       <c r="D20" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="69" t="s">
+      <c r="E20" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
       <c r="H20" s="45">
         <v>42841</v>
       </c>
@@ -4897,7 +4891,7 @@
         <v>234</v>
       </c>
       <c r="N20" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O20" s="27"/>
     </row>
@@ -4912,11 +4906,11 @@
       <c r="D21" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="69" t="s">
+      <c r="E21" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="45">
         <v>42841</v>
       </c>
@@ -4936,7 +4930,7 @@
         <v>234</v>
       </c>
       <c r="N21" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O21" s="27"/>
     </row>
@@ -4951,11 +4945,11 @@
       <c r="D22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
       <c r="H22" s="45">
         <v>42841</v>
       </c>
@@ -4973,7 +4967,7 @@
         <v>234</v>
       </c>
       <c r="N22" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O22" s="27"/>
     </row>
@@ -4988,11 +4982,11 @@
       <c r="D23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
       <c r="H23" s="45">
         <v>42841</v>
       </c>
@@ -5012,7 +5006,7 @@
         <v>234</v>
       </c>
       <c r="N23" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O23" s="27"/>
     </row>
@@ -5027,11 +5021,11 @@
       <c r="D24" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="59" t="s">
         <v>207</v>
       </c>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
       <c r="H24" s="45">
         <v>42841</v>
       </c>
@@ -5049,7 +5043,7 @@
         <v>234</v>
       </c>
       <c r="N24" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O24" s="27"/>
     </row>
@@ -5064,11 +5058,11 @@
       <c r="D25" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
       <c r="H25" s="45">
         <v>42841</v>
       </c>
@@ -5088,7 +5082,7 @@
         <v>234</v>
       </c>
       <c r="N25" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O25" s="27"/>
     </row>
@@ -5103,11 +5097,11 @@
       <c r="D26" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="57" t="s">
+      <c r="E26" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
       <c r="H26" s="45">
         <v>42841</v>
       </c>
@@ -5125,7 +5119,7 @@
         <v>234</v>
       </c>
       <c r="N26" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O26" s="27"/>
     </row>
@@ -5140,11 +5134,11 @@
       <c r="D27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="69" t="s">
+      <c r="E27" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
       <c r="H27" s="45">
         <v>42841</v>
       </c>
@@ -5162,7 +5156,7 @@
         <v>234</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O27" s="27"/>
     </row>
@@ -5177,11 +5171,11 @@
       <c r="D28" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
       <c r="H28" s="45">
         <v>42841</v>
       </c>
@@ -5201,7 +5195,7 @@
         <v>234</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O28" s="31"/>
     </row>
@@ -5216,11 +5210,11 @@
       <c r="D29" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
       <c r="H29" s="45">
         <v>42841</v>
       </c>
@@ -5240,7 +5234,7 @@
         <v>234</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="40"/>
@@ -5259,11 +5253,11 @@
       <c r="D30" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="45">
         <v>42841</v>
       </c>
@@ -5281,7 +5275,7 @@
         <v>234</v>
       </c>
       <c r="N30" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O30" s="31"/>
     </row>
@@ -5296,11 +5290,11 @@
       <c r="D31" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
       <c r="H31" s="45">
         <v>42841</v>
       </c>
@@ -5318,7 +5312,7 @@
         <v>234</v>
       </c>
       <c r="N31" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O31" s="31"/>
     </row>
@@ -5333,11 +5327,11 @@
       <c r="D32" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
       <c r="H32" s="45">
         <v>42841</v>
       </c>
@@ -5355,7 +5349,7 @@
         <v>234</v>
       </c>
       <c r="N32" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O32" s="31"/>
     </row>
@@ -5370,11 +5364,11 @@
       <c r="D33" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="57" t="s">
+      <c r="E33" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="45">
         <v>42841</v>
       </c>
@@ -5392,7 +5386,7 @@
         <v>234</v>
       </c>
       <c r="N33" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O33" s="31"/>
     </row>
@@ -5407,11 +5401,11 @@
       <c r="D34" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="E34" s="57" t="s">
+      <c r="E34" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
       <c r="H34" s="45">
         <v>42841</v>
       </c>
@@ -5429,7 +5423,7 @@
         <v>234</v>
       </c>
       <c r="N34" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O34" s="31"/>
     </row>
@@ -5444,11 +5438,11 @@
       <c r="D35" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="E35" s="57" t="s">
+      <c r="E35" s="59" t="s">
         <v>247</v>
       </c>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
       <c r="H35" s="45">
         <v>42841</v>
       </c>
@@ -5466,7 +5460,7 @@
         <v>234</v>
       </c>
       <c r="N35" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O35" s="31"/>
     </row>
@@ -5481,11 +5475,11 @@
       <c r="D36" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
       <c r="H36" s="45">
         <v>42841</v>
       </c>
@@ -5503,84 +5497,84 @@
         <v>234</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O36" s="31"/>
     </row>
-    <row r="37" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
-      <c r="A37" s="51" t="s">
-        <v>251</v>
-      </c>
-      <c r="B37" s="39" t="s">
-        <v>252</v>
-      </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="57" t="s">
-        <v>250</v>
-      </c>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="45">
-        <v>42841</v>
-      </c>
-      <c r="I37" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="37"/>
-      <c r="K37" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L37" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M37" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="N37" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="O37" s="31"/>
-    </row>
-    <row r="38" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A38" s="59" t="s">
+    <row r="37" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A37" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
+      <c r="N37" s="70"/>
+      <c r="O37" s="71"/>
+    </row>
+    <row r="38" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+      <c r="A38" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="59" t="s">
+        <v>61</v>
+      </c>
       <c r="F38" s="60"/>
       <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="61"/>
-    </row>
-    <row r="39" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+      <c r="H38" s="45">
+        <v>42843</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="37"/>
+      <c r="K38" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L38" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M38" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="N38" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="O38" s="31"/>
+    </row>
+    <row r="39" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A39" s="29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>212</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C39" s="31"/>
       <c r="D39" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
+        <v>70</v>
+      </c>
+      <c r="E39" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
       <c r="H39" s="45">
         <v>42843</v>
       </c>
@@ -5589,7 +5583,7 @@
       </c>
       <c r="J39" s="37"/>
       <c r="K39" s="54" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L39" s="28" t="s">
         <v>18</v>
@@ -5598,26 +5592,28 @@
         <v>234</v>
       </c>
       <c r="N39" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O39" s="31"/>
     </row>
-    <row r="40" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
+    <row r="40" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A40" s="29" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="31"/>
+        <v>63</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="D40" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
+        <v>71</v>
+      </c>
+      <c r="E40" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
       <c r="H40" s="45">
         <v>42843</v>
       </c>
@@ -5635,28 +5631,28 @@
         <v>234</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O40" s="31"/>
     </row>
-    <row r="41" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="41" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A41" s="29" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
       <c r="H41" s="45">
         <v>42843</v>
       </c>
@@ -5674,30 +5670,28 @@
         <v>234</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O41" s="31"/>
     </row>
-    <row r="42" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="42" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A42" s="29" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>66</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="C42" s="31"/>
       <c r="D42" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
+        <v>215</v>
+      </c>
+      <c r="E42" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
       <c r="H42" s="45">
-        <v>42843</v>
+        <v>42869</v>
       </c>
       <c r="I42" s="54" t="s">
         <v>13</v>
@@ -5713,28 +5707,30 @@
         <v>234</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O42" s="31"/>
     </row>
     <row r="43" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A43" s="29" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="C43" s="31"/>
+        <v>127</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>109</v>
+      </c>
       <c r="D43" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="E43" s="57" t="s">
-        <v>216</v>
-      </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
+        <v>128</v>
+      </c>
+      <c r="E43" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
       <c r="H43" s="45">
-        <v>42869</v>
+        <v>42843</v>
       </c>
       <c r="I43" s="54" t="s">
         <v>13</v>
@@ -5746,90 +5742,90 @@
       <c r="L43" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M43" s="50" t="s">
+      <c r="M43" s="52" t="s">
         <v>234</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O43" s="31"/>
     </row>
-    <row r="44" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
-      <c r="A44" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" s="31" t="s">
+    <row r="44" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A44" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="70"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="70"/>
+      <c r="J44" s="70"/>
+      <c r="K44" s="70"/>
+      <c r="L44" s="70"/>
+      <c r="M44" s="70"/>
+      <c r="N44" s="70"/>
+      <c r="O44" s="71"/>
+    </row>
+    <row r="45" spans="1:15" s="30" customFormat="1" ht="140.25" outlineLevel="1">
+      <c r="A45" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="57" t="s">
-        <v>129</v>
-      </c>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="45">
-        <v>42843</v>
-      </c>
-      <c r="I44" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" s="37"/>
-      <c r="K44" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L44" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M44" s="52" t="s">
-        <v>234</v>
-      </c>
-      <c r="N44" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="O44" s="31"/>
-    </row>
-    <row r="45" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A45" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
+      <c r="D45" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="59" t="s">
+        <v>132</v>
+      </c>
       <c r="F45" s="60"/>
       <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
-      <c r="N45" s="60"/>
-      <c r="O45" s="61"/>
-    </row>
-    <row r="46" spans="1:15" s="30" customFormat="1" ht="140.25" outlineLevel="1">
+      <c r="H45" s="45">
+        <v>42843</v>
+      </c>
+      <c r="I45" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" s="37"/>
+      <c r="K45" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L45" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M45" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="N45" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="O45" s="31"/>
+    </row>
+    <row r="46" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A46" s="29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C46" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="57" t="s">
-        <v>132</v>
-      </c>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
+        <v>77</v>
+      </c>
+      <c r="E46" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
       <c r="H46" s="45">
         <v>42843</v>
       </c>
@@ -5838,7 +5834,7 @@
       </c>
       <c r="J46" s="37"/>
       <c r="K46" s="54" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L46" s="28" t="s">
         <v>18</v>
@@ -5847,28 +5843,28 @@
         <v>234</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O46" s="31"/>
     </row>
-    <row r="47" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
+    <row r="47" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A47" s="29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C47" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
       <c r="H47" s="45">
         <v>42843</v>
       </c>
@@ -5886,35 +5882,37 @@
         <v>234</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O47" s="31"/>
     </row>
     <row r="48" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A48" s="29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C48" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E48" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
+        <v>81</v>
+      </c>
+      <c r="E48" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
       <c r="H48" s="45">
         <v>42843</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="37"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="46" t="s">
+        <v>151</v>
+      </c>
       <c r="K48" s="54" t="s">
         <v>161</v>
       </c>
@@ -5925,37 +5923,35 @@
         <v>234</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O48" s="31"/>
     </row>
-    <row r="49" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="49" spans="1:15" s="30" customFormat="1" ht="102" outlineLevel="1">
       <c r="A49" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="C49" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
+        <v>137</v>
+      </c>
+      <c r="E49" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
       <c r="H49" s="45">
         <v>42843</v>
       </c>
       <c r="I49" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J49" s="46" t="s">
-        <v>151</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J49" s="46"/>
       <c r="K49" s="54" t="s">
         <v>161</v>
       </c>
@@ -5966,35 +5962,37 @@
         <v>234</v>
       </c>
       <c r="N49" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O49" s="31"/>
     </row>
-    <row r="50" spans="1:15" s="30" customFormat="1" ht="102" outlineLevel="1">
+    <row r="50" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A50" s="29" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="C50" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E50" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
+        <v>82</v>
+      </c>
+      <c r="E50" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
       <c r="H50" s="45">
         <v>42843</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J50" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="46" t="s">
+        <v>151</v>
+      </c>
       <c r="K50" s="54" t="s">
         <v>161</v>
       </c>
@@ -6005,28 +6003,28 @@
         <v>234</v>
       </c>
       <c r="N50" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O50" s="31"/>
     </row>
     <row r="51" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A51" s="29" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C51" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
+        <v>86</v>
+      </c>
+      <c r="E51" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
       <c r="H51" s="45">
         <v>42843</v>
       </c>
@@ -6034,7 +6032,7 @@
         <v>0</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K51" s="54" t="s">
         <v>161</v>
@@ -6043,98 +6041,98 @@
         <v>18</v>
       </c>
       <c r="M51" s="50" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="N51" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O51" s="31"/>
     </row>
-    <row r="52" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
-      <c r="A52" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="B52" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E52" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="45">
-        <v>42843</v>
-      </c>
-      <c r="I52" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J52" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="K52" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="L52" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M52" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="N52" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="O52" s="31"/>
-    </row>
-    <row r="53" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A53" s="59" t="s">
+    <row r="52" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A52" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="70"/>
+      <c r="K52" s="70"/>
+      <c r="L52" s="70"/>
+      <c r="M52" s="70"/>
+      <c r="N52" s="70"/>
+      <c r="O52" s="71"/>
+    </row>
+    <row r="53" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
+      <c r="A53" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="59" t="s">
+        <v>149</v>
+      </c>
       <c r="F53" s="60"/>
       <c r="G53" s="60"/>
-      <c r="H53" s="60"/>
-      <c r="I53" s="60"/>
-      <c r="J53" s="60"/>
-      <c r="K53" s="60"/>
-      <c r="L53" s="60"/>
-      <c r="M53" s="60"/>
-      <c r="N53" s="60"/>
-      <c r="O53" s="61"/>
-    </row>
-    <row r="54" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
+      <c r="H53" s="45">
+        <v>42843</v>
+      </c>
+      <c r="I53" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="37"/>
+      <c r="K53" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="L53" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M53" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="N53" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="O53" s="31"/>
+    </row>
+    <row r="54" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A54" s="29" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E54" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
+        <v>102</v>
+      </c>
+      <c r="E54" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
       <c r="H54" s="45">
         <v>42843</v>
       </c>
       <c r="I54" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="37"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="46" t="s">
+        <v>150</v>
+      </c>
       <c r="K54" s="54" t="s">
         <v>161</v>
       </c>
@@ -6142,40 +6140,38 @@
         <v>18</v>
       </c>
       <c r="M54" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N54" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O54" s="31"/>
     </row>
     <row r="55" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A55" s="29" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
+        <v>144</v>
+      </c>
+      <c r="E55" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
       <c r="H55" s="45">
         <v>42843</v>
       </c>
       <c r="I55" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J55" s="46" t="s">
-        <v>150</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J55" s="37"/>
       <c r="K55" s="54" t="s">
         <v>161</v>
       </c>
@@ -6183,38 +6179,40 @@
         <v>18</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N55" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O55" s="31"/>
     </row>
-    <row r="56" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
+    <row r="56" spans="1:15" s="30" customFormat="1" ht="127.5" outlineLevel="1">
       <c r="A56" s="29" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="C56" s="31" t="s">
         <v>108</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
+        <v>139</v>
+      </c>
+      <c r="E56" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
       <c r="H56" s="45">
         <v>42843</v>
       </c>
       <c r="I56" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J56" s="37"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="46" t="s">
+        <v>150</v>
+      </c>
       <c r="K56" s="54" t="s">
         <v>161</v>
       </c>
@@ -6222,31 +6220,31 @@
         <v>18</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N56" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O56" s="31"/>
     </row>
-    <row r="57" spans="1:15" s="30" customFormat="1" ht="127.5" outlineLevel="1">
+    <row r="57" spans="1:15" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A57" s="29" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="31" t="s">
         <v>108</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="E57" s="57" t="s">
-        <v>147</v>
-      </c>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
+        <v>140</v>
+      </c>
+      <c r="E57" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
       <c r="H57" s="45">
         <v>42843</v>
       </c>
@@ -6254,7 +6252,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K57" s="54" t="s">
         <v>161</v>
@@ -6263,40 +6261,38 @@
         <v>18</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N57" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O57" s="31"/>
     </row>
-    <row r="58" spans="1:15" s="30" customFormat="1" ht="114.75" outlineLevel="1">
+    <row r="58" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A58" s="29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
+        <v>153</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
       <c r="H58" s="45">
         <v>42843</v>
       </c>
       <c r="I58" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J58" s="46" t="s">
-        <v>148</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J58" s="46"/>
       <c r="K58" s="54" t="s">
         <v>161</v>
       </c>
@@ -6304,70 +6300,72 @@
         <v>18</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N58" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O58" s="31"/>
     </row>
-    <row r="59" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="59" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A59" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
+        <v>96</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
       <c r="H59" s="45">
         <v>42843</v>
       </c>
       <c r="I59" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J59" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="46" t="s">
+        <v>92</v>
+      </c>
       <c r="K59" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L59" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N59" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O59" s="31"/>
     </row>
-    <row r="60" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="60" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A60" s="29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C60" s="31" t="s">
         <v>106</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E60" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
+        <v>95</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>97</v>
+      </c>
+      <c r="F60" s="60"/>
+      <c r="G60" s="60"/>
       <c r="H60" s="45">
         <v>42843</v>
       </c>
@@ -6375,7 +6373,7 @@
         <v>0</v>
       </c>
       <c r="J60" s="46" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="K60" s="54" t="s">
         <v>160</v>
@@ -6384,79 +6382,77 @@
         <v>18</v>
       </c>
       <c r="M60" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N60" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O60" s="31"/>
     </row>
-    <row r="61" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="61" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A61" s="29" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E61" s="57" t="s">
-        <v>97</v>
-      </c>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
+        <v>101</v>
+      </c>
+      <c r="E61" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
       <c r="H61" s="45">
         <v>42843</v>
       </c>
       <c r="I61" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J61" s="46" t="s">
-        <v>99</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J61" s="46"/>
       <c r="K61" s="54" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L61" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M61" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N61" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O61" s="31"/>
     </row>
-    <row r="62" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
+    <row r="62" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A62" s="29" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="F62" s="58"/>
-      <c r="G62" s="58"/>
+        <v>141</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="F62" s="60"/>
+      <c r="G62" s="60"/>
       <c r="H62" s="45">
         <v>42843</v>
       </c>
       <c r="I62" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J62" s="46"/>
+      <c r="J62" s="37"/>
       <c r="K62" s="54" t="s">
         <v>161</v>
       </c>
@@ -6464,38 +6460,38 @@
         <v>18</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N62" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O62" s="31"/>
     </row>
-    <row r="63" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
+    <row r="63" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A63" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>110</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="E63" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
+        <v>155</v>
+      </c>
+      <c r="E63" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" s="60"/>
+      <c r="G63" s="60"/>
       <c r="H63" s="45">
         <v>42843</v>
       </c>
       <c r="I63" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J63" s="37"/>
+      <c r="J63" s="46"/>
       <c r="K63" s="54" t="s">
         <v>161</v>
       </c>
@@ -6503,89 +6499,89 @@
         <v>18</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N63" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O63" s="31"/>
     </row>
-    <row r="64" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A64" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B64" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E64" s="57" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" s="58"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="45">
-        <v>42843</v>
-      </c>
-      <c r="I64" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J64" s="46"/>
-      <c r="K64" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="L64" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M64" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="N64" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="O64" s="31"/>
-    </row>
-    <row r="65" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A65" s="59" t="s">
+    <row r="64" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A64" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="B65" s="60"/>
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
+      <c r="B64" s="70"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="70"/>
+      <c r="F64" s="70"/>
+      <c r="G64" s="70"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="70"/>
+      <c r="K64" s="70"/>
+      <c r="L64" s="70"/>
+      <c r="M64" s="70"/>
+      <c r="N64" s="70"/>
+      <c r="O64" s="71"/>
+    </row>
+    <row r="65" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="A65" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>116</v>
+      </c>
       <c r="F65" s="60"/>
       <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
-      <c r="J65" s="60"/>
-      <c r="K65" s="60"/>
-      <c r="L65" s="60"/>
-      <c r="M65" s="60"/>
-      <c r="N65" s="60"/>
-      <c r="O65" s="61"/>
-    </row>
-    <row r="66" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="H65" s="45">
+        <v>42847</v>
+      </c>
+      <c r="I65" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="46"/>
+      <c r="K65" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="L65" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M65" s="50" t="s">
+        <v>257</v>
+      </c>
+      <c r="N65" s="50" t="s">
+        <v>254</v>
+      </c>
+      <c r="O65" s="31"/>
+    </row>
+    <row r="66" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A66" s="29" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="E66" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="F66" s="58"/>
-      <c r="G66" s="58"/>
+        <v>120</v>
+      </c>
+      <c r="E66" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
       <c r="H66" s="45">
         <v>42847</v>
       </c>
@@ -6600,31 +6596,31 @@
         <v>18</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N66" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O66" s="31"/>
     </row>
-    <row r="67" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="67" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A67" s="29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>118</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E67" s="57" t="s">
-        <v>156</v>
-      </c>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
+        <v>157</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="F67" s="60"/>
+      <c r="G67" s="60"/>
       <c r="H67" s="45">
         <v>42847</v>
       </c>
@@ -6639,38 +6635,40 @@
         <v>18</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N67" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O67" s="31"/>
     </row>
     <row r="68" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A68" s="29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="E68" s="57" t="s">
-        <v>158</v>
-      </c>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
+        <v>123</v>
+      </c>
+      <c r="E68" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F68" s="60"/>
+      <c r="G68" s="60"/>
       <c r="H68" s="45">
         <v>42847</v>
       </c>
       <c r="I68" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J68" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J68" s="46" t="s">
+        <v>125</v>
+      </c>
       <c r="K68" s="54" t="s">
         <v>160</v>
       </c>
@@ -6678,16 +6676,16 @@
         <v>18</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N68" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O68" s="31"/>
     </row>
     <row r="69" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A69" s="29" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B69" s="39" t="s">
         <v>121</v>
@@ -6698,20 +6696,18 @@
       <c r="D69" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="E69" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="F69" s="58"/>
-      <c r="G69" s="58"/>
+      <c r="E69" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" s="60"/>
+      <c r="G69" s="60"/>
       <c r="H69" s="45">
         <v>42847</v>
       </c>
       <c r="I69" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J69" s="46" t="s">
-        <v>125</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J69" s="46"/>
       <c r="K69" s="54" t="s">
         <v>160</v>
       </c>
@@ -6719,51 +6715,23 @@
         <v>18</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="N69" s="50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O69" s="31"/>
     </row>
-    <row r="70" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A70" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="B70" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="C70" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D70" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="E70" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="45">
-        <v>42847</v>
-      </c>
-      <c r="I70" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J70" s="46"/>
-      <c r="K70" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L70" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M70" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="N70" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="O70" s="31"/>
+    <row r="70" spans="1:15" ht="12" customHeight="1">
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="I70" s="55"/>
+      <c r="J70"/>
+      <c r="K70" s="55"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
     </row>
     <row r="71" spans="1:15" ht="12" customHeight="1">
       <c r="B71"/>
@@ -6864,9 +6832,7 @@
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="1:15" ht="12" customHeight="1">
-      <c r="B80"/>
-      <c r="C80"/>
+    <row r="80" spans="1:15" ht="13.5">
       <c r="I80" s="55"/>
       <c r="J80"/>
       <c r="K80" s="55"/>
@@ -11132,25 +11098,65 @@
       <c r="N553"/>
       <c r="O553"/>
     </row>
-    <row r="554" spans="9:15" ht="13.5">
-      <c r="I554" s="55"/>
-      <c r="J554"/>
-      <c r="K554" s="55"/>
-      <c r="L554"/>
-      <c r="M554"/>
-      <c r="N554"/>
-      <c r="O554"/>
-    </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
+  <mergeCells count="81">
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="A64:O64"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="A52:O52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="A44:O44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:G10"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="B1:E2"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -11167,93 +11173,43 @@
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A38:O38"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:G10"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A45:O45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="A53:O53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="A65:O65"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Automated">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Not">
+      <formula>LEFT(M1,LEN("Not"))="Not"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",M1)))</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="Not">
-      <formula>LEFT(M1,LEN("Not"))="Not"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M54:M64 M39:M44 M13:M16 M18:M37 M46:M52 M66:M70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M53:M63 M38:M43 M13:M16 M18:M36 M45:M51 M65:M69">
       <formula1>$S$1:$S$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N37 N39:N44 N46:N52 N54:N64 N66:N70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N53:N63 N65:N69">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I37 I39:I44 I46:I52 I55:I64 I66:I70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I54:I63 I65:I69">
       <formula1>$R$1:$R$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K37 K39:K44 K46:K52 K54:K64 K66:K70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K53:K63 K65:K69">
       <formula1>$Q$1:$Q$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Separate test cases for edit and delete article
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="259">
   <si>
     <t>Fail</t>
   </si>
@@ -401,9 +401,6 @@
 4: Click on "Create" button</t>
   </si>
   <si>
-    <t>4. Tests on "Edit and Delete Article" page</t>
-  </si>
-  <si>
     <t>Edit Article with valid data</t>
   </si>
   <si>
@@ -763,39 +760,6 @@
     <t>CAP_TC7</t>
   </si>
   <si>
-    <t>EDAP_TC1</t>
-  </si>
-  <si>
-    <t>EDAP_TC2</t>
-  </si>
-  <si>
-    <t>EDAP_TC3</t>
-  </si>
-  <si>
-    <t>EDAP_TC4</t>
-  </si>
-  <si>
-    <t>EDAP_TC5</t>
-  </si>
-  <si>
-    <t>EDAP_TC6</t>
-  </si>
-  <si>
-    <t>EDAP_TC7</t>
-  </si>
-  <si>
-    <t>EDAP_TC8</t>
-  </si>
-  <si>
-    <t>EDAP_TC9</t>
-  </si>
-  <si>
-    <t>EDAP_TC11</t>
-  </si>
-  <si>
-    <t>EDAP_TC10</t>
-  </si>
-  <si>
     <t>EDUP_TC1</t>
   </si>
   <si>
@@ -809,9 +773,6 @@
   </si>
   <si>
     <t>EDUP_TC5</t>
-  </si>
-  <si>
-    <t>5. Tests on  "Edit Users" page</t>
   </si>
   <si>
     <t>Register with name longer than 50 characters</t>
@@ -1003,6 +964,48 @@
   </si>
   <si>
     <t>Not Atomated</t>
+  </si>
+  <si>
+    <t>EAP_TC1</t>
+  </si>
+  <si>
+    <t>4. Tests on "Edit Article" page</t>
+  </si>
+  <si>
+    <t>5. Tests on "Delete Article" page</t>
+  </si>
+  <si>
+    <t>6. Tests on  "Edit Users" page</t>
+  </si>
+  <si>
+    <t>EAP_TC2</t>
+  </si>
+  <si>
+    <t>EAP_TC3</t>
+  </si>
+  <si>
+    <t>EAP_TC4</t>
+  </si>
+  <si>
+    <t>EAP_TC5</t>
+  </si>
+  <si>
+    <t>DAP_TC3</t>
+  </si>
+  <si>
+    <t>DAP_TC2</t>
+  </si>
+  <si>
+    <t>DAP_TC1</t>
+  </si>
+  <si>
+    <t>EAP_TC6</t>
+  </si>
+  <si>
+    <t>EAP_TC7</t>
+  </si>
+  <si>
+    <t>EAP_TC8</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1672,55 @@
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1"/>
     <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="2"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -4291,12 +4342,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T553"/>
+  <dimension ref="A1:T554"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="A37" sqref="A37:XFD37"/>
+      <selection pane="topRight" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4335,16 +4386,16 @@
       <c r="O1" s="43"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
@@ -4365,16 +4416,16 @@
       <c r="O2" s="43"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4399,10 +4450,10 @@
       <c r="O3" s="73"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="25.5">
@@ -4425,7 +4476,7 @@
       <c r="O4" s="73"/>
       <c r="P4" s="7"/>
       <c r="T4" s="2" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="23" customFormat="1" ht="25.5">
@@ -4448,7 +4499,7 @@
       <c r="O5" s="72"/>
       <c r="P5" s="22"/>
       <c r="T5" s="23" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4456,7 +4507,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="32">
-        <f>COUNTIF(I17:I137,"Pass")</f>
+        <f>COUNTIF(I17:I138,"Pass")</f>
         <v>34</v>
       </c>
       <c r="C6" s="32"/>
@@ -4464,7 +4515,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="10">
-        <f>COUNTIF(I10:I760,"Pending")</f>
+        <f>COUNTIF(I10:I761,"Pending")</f>
         <v>0</v>
       </c>
       <c r="F6" s="6"/>
@@ -4484,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="33">
-        <f>COUNTIF(I17:I137,"Fail")</f>
+        <f>COUNTIF(I17:I138,"Fail")</f>
         <v>14</v>
       </c>
       <c r="C7" s="33"/>
@@ -4492,7 +4543,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF(A17:A137,"TC*")</f>
+        <f>COUNTIF(A17:A138,"TC*")</f>
         <v>0</v>
       </c>
       <c r="F7" s="17"/>
@@ -4553,16 +4604,16 @@
         <v>16</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L9" s="57" t="s">
         <v>17</v>
       </c>
       <c r="M9" s="57" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="N9" s="57" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="O9" s="76" t="s">
         <v>10</v>
@@ -4606,7 +4657,7 @@
     </row>
     <row r="12" spans="1:20" s="3" customFormat="1" ht="12.75">
       <c r="A12" s="69" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
@@ -4625,17 +4676,17 @@
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="76.5" customHeight="1" outlineLevel="1">
       <c r="A13" s="29" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="28" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
@@ -4647,32 +4698,32 @@
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N13" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:20" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A14" s="29" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="28" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
@@ -4684,30 +4735,30 @@
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L14" s="28"/>
       <c r="M14" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N14" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A15" s="29" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="28" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
@@ -4719,30 +4770,30 @@
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L15" s="28"/>
       <c r="M15" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N15" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A16" s="29" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="28" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="F16" s="62"/>
       <c r="G16" s="62"/>
@@ -4754,14 +4805,14 @@
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L16" s="28"/>
       <c r="M16" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N16" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O16" s="27"/>
     </row>
@@ -4786,17 +4837,17 @@
     </row>
     <row r="18" spans="1:19" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A18" s="29" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="28" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F18" s="62"/>
       <c r="G18" s="62"/>
@@ -4808,22 +4859,22 @@
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N18" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A19" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>15</v>
@@ -4833,7 +4884,7 @@
         <v>58</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F19" s="62"/>
       <c r="G19" s="62"/>
@@ -4845,22 +4896,22 @@
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N19" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A20" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>19</v>
@@ -4882,22 +4933,22 @@
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L20" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N20" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A21" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>21</v>
@@ -4921,22 +4972,22 @@
         <v>24</v>
       </c>
       <c r="K21" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L21" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N21" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:19" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A22" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B22" s="39" t="s">
         <v>25</v>
@@ -4958,22 +5009,22 @@
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L22" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N22" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O22" s="27"/>
     </row>
     <row r="23" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A23" s="29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>27</v>
@@ -4997,32 +5048,32 @@
         <v>30</v>
       </c>
       <c r="K23" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L23" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N23" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A24" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="28" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F24" s="60"/>
       <c r="G24" s="60"/>
@@ -5034,22 +5085,22 @@
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N24" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" s="39" t="s">
         <v>34</v>
@@ -5073,22 +5124,22 @@
         <v>32</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L25" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N25" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B26" s="39" t="s">
         <v>33</v>
@@ -5110,22 +5161,22 @@
       </c>
       <c r="J26" s="28"/>
       <c r="K26" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L26" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N26" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A27" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>37</v>
@@ -5147,22 +5198,22 @@
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L27" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A28" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B28" s="39" t="s">
         <v>40</v>
@@ -5186,32 +5237,32 @@
         <v>30</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L28" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O28" s="31"/>
     </row>
     <row r="29" spans="1:19" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A29" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="28" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E29" s="59" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="F29" s="60"/>
       <c r="G29" s="60"/>
@@ -5225,16 +5276,16 @@
         <v>32</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L29" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="40"/>
@@ -5244,7 +5295,7 @@
     </row>
     <row r="30" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A30" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="39" t="s">
         <v>43</v>
@@ -5266,22 +5317,22 @@
       </c>
       <c r="J30" s="37"/>
       <c r="K30" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L30" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N30" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O30" s="31"/>
     </row>
     <row r="31" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A31" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="39" t="s">
         <v>47</v>
@@ -5303,22 +5354,22 @@
       </c>
       <c r="J31" s="37"/>
       <c r="K31" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N31" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O31" s="31"/>
     </row>
     <row r="32" spans="1:19" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A32" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>51</v>
@@ -5340,22 +5391,22 @@
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L32" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N32" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O32" s="31"/>
     </row>
     <row r="33" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A33" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B33" s="39" t="s">
         <v>54</v>
@@ -5377,32 +5428,32 @@
       </c>
       <c r="J33" s="37"/>
       <c r="K33" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L33" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M33" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N33" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O33" s="31"/>
     </row>
     <row r="34" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A34" s="51" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C34" s="39"/>
       <c r="D34" s="28" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E34" s="59" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="F34" s="60"/>
       <c r="G34" s="60"/>
@@ -5414,32 +5465,32 @@
       </c>
       <c r="J34" s="37"/>
       <c r="K34" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L34" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M34" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N34" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O34" s="31"/>
     </row>
     <row r="35" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A35" s="51" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C35" s="39"/>
       <c r="D35" s="28" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="E35" s="59" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="F35" s="60"/>
       <c r="G35" s="60"/>
@@ -5451,32 +5502,32 @@
       </c>
       <c r="J35" s="37"/>
       <c r="K35" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L35" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M35" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N35" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O35" s="31"/>
     </row>
     <row r="36" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A36" s="51" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C36" s="39"/>
       <c r="D36" s="28" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E36" s="59" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="F36" s="60"/>
       <c r="G36" s="60"/>
@@ -5488,16 +5539,16 @@
       </c>
       <c r="J36" s="37"/>
       <c r="K36" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L36" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M36" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O36" s="31"/>
     </row>
@@ -5522,13 +5573,13 @@
     </row>
     <row r="38" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A38" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>69</v>
@@ -5546,22 +5597,22 @@
       </c>
       <c r="J38" s="37"/>
       <c r="K38" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L38" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M38" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N38" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O38" s="31"/>
     </row>
     <row r="39" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A39" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>62</v>
@@ -5583,22 +5634,22 @@
       </c>
       <c r="J39" s="37"/>
       <c r="K39" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L39" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M39" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N39" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O39" s="31"/>
     </row>
     <row r="40" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A40" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B40" s="39" t="s">
         <v>63</v>
@@ -5610,7 +5661,7 @@
         <v>71</v>
       </c>
       <c r="E40" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F40" s="60"/>
       <c r="G40" s="60"/>
@@ -5622,22 +5673,22 @@
       </c>
       <c r="J40" s="37"/>
       <c r="K40" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L40" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M40" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O40" s="31"/>
     </row>
     <row r="41" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A41" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B41" s="39" t="s">
         <v>64</v>
@@ -5649,7 +5700,7 @@
         <v>72</v>
       </c>
       <c r="E41" s="59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F41" s="60"/>
       <c r="G41" s="60"/>
@@ -5661,32 +5712,32 @@
       </c>
       <c r="J41" s="37"/>
       <c r="K41" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L41" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M41" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O41" s="31"/>
     </row>
     <row r="42" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A42" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="28" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E42" s="59" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="F42" s="60"/>
       <c r="G42" s="60"/>
@@ -5698,34 +5749,34 @@
       </c>
       <c r="J42" s="37"/>
       <c r="K42" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L42" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M42" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O42" s="31"/>
     </row>
     <row r="43" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A43" s="29" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B43" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="28" t="s">
+      <c r="E43" s="59" t="s">
         <v>128</v>
-      </c>
-      <c r="E43" s="59" t="s">
-        <v>129</v>
       </c>
       <c r="F43" s="60"/>
       <c r="G43" s="60"/>
@@ -5737,16 +5788,16 @@
       </c>
       <c r="J43" s="37"/>
       <c r="K43" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L43" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M43" s="52" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O43" s="31"/>
     </row>
@@ -5771,19 +5822,19 @@
     </row>
     <row r="45" spans="1:15" s="30" customFormat="1" ht="140.25" outlineLevel="1">
       <c r="A45" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B45" s="39" t="s">
         <v>68</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E45" s="59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F45" s="60"/>
       <c r="G45" s="60"/>
@@ -5795,34 +5846,34 @@
       </c>
       <c r="J45" s="37"/>
       <c r="K45" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L45" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M45" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N45" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O45" s="31"/>
     </row>
     <row r="46" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A46" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B46" s="39" t="s">
         <v>76</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F46" s="60"/>
       <c r="G46" s="60"/>
@@ -5834,34 +5885,34 @@
       </c>
       <c r="J46" s="37"/>
       <c r="K46" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L46" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M46" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O46" s="31"/>
     </row>
     <row r="47" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A47" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B47" s="39" t="s">
         <v>79</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" s="28" t="s">
         <v>80</v>
       </c>
       <c r="E47" s="59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F47" s="60"/>
       <c r="G47" s="60"/>
@@ -5873,34 +5924,34 @@
       </c>
       <c r="J47" s="37"/>
       <c r="K47" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L47" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M47" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O47" s="31"/>
     </row>
     <row r="48" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A48" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" s="39" t="s">
         <v>83</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D48" s="28" t="s">
         <v>81</v>
       </c>
       <c r="E48" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F48" s="60"/>
       <c r="G48" s="60"/>
@@ -5911,37 +5962,37 @@
         <v>0</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K48" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L48" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M48" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O48" s="31"/>
     </row>
     <row r="49" spans="1:15" s="30" customFormat="1" ht="102" outlineLevel="1">
       <c r="A49" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F49" s="60"/>
       <c r="G49" s="60"/>
@@ -5953,34 +6004,34 @@
       </c>
       <c r="J49" s="46"/>
       <c r="K49" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L49" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M49" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N49" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O49" s="31"/>
     </row>
     <row r="50" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A50" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B50" s="39" t="s">
         <v>84</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D50" s="28" t="s">
         <v>82</v>
       </c>
       <c r="E50" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F50" s="60"/>
       <c r="G50" s="60"/>
@@ -5991,37 +6042,37 @@
         <v>0</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K50" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L50" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="50" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="N50" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O50" s="31"/>
     </row>
     <row r="51" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A51" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51" s="39" t="s">
         <v>85</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" s="28" t="s">
         <v>86</v>
       </c>
       <c r="E51" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F51" s="60"/>
       <c r="G51" s="60"/>
@@ -6032,25 +6083,25 @@
         <v>0</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K51" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L51" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M51" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N51" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="1:15" s="3" customFormat="1" ht="12.75">
       <c r="A52" s="69" t="s">
-        <v>87</v>
+        <v>246</v>
       </c>
       <c r="B52" s="70"/>
       <c r="C52" s="70"/>
@@ -6069,19 +6120,19 @@
     </row>
     <row r="53" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
       <c r="A53" s="29" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E53" s="59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F53" s="60"/>
       <c r="G53" s="60"/>
@@ -6093,34 +6144,34 @@
       </c>
       <c r="J53" s="37"/>
       <c r="K53" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L53" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M53" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N53" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O53" s="31"/>
     </row>
     <row r="54" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A54" s="29" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F54" s="60"/>
       <c r="G54" s="60"/>
@@ -6131,37 +6182,37 @@
         <v>0</v>
       </c>
       <c r="J54" s="46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K54" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L54" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M54" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N54" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O54" s="31"/>
     </row>
     <row r="55" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A55" s="29" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="B55" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>144</v>
-      </c>
       <c r="E55" s="59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F55" s="60"/>
       <c r="G55" s="60"/>
@@ -6173,34 +6224,34 @@
       </c>
       <c r="J55" s="37"/>
       <c r="K55" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L55" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N55" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O55" s="31"/>
     </row>
     <row r="56" spans="1:15" s="30" customFormat="1" ht="127.5" outlineLevel="1">
       <c r="A56" s="29" t="s">
-        <v>192</v>
+        <v>251</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E56" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F56" s="60"/>
       <c r="G56" s="60"/>
@@ -6211,37 +6262,37 @@
         <v>0</v>
       </c>
       <c r="J56" s="46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K56" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L56" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N56" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O56" s="31"/>
     </row>
     <row r="57" spans="1:15" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A57" s="29" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E57" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F57" s="60"/>
       <c r="G57" s="60"/>
@@ -6252,37 +6303,37 @@
         <v>0</v>
       </c>
       <c r="J57" s="46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K57" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L57" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N57" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O57" s="31"/>
     </row>
-    <row r="58" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="58" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A58" s="29" t="s">
-        <v>194</v>
+        <v>256</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="E58" s="59" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="F58" s="60"/>
       <c r="G58" s="60"/>
@@ -6294,34 +6345,34 @@
       </c>
       <c r="J58" s="46"/>
       <c r="K58" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L58" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N58" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O58" s="31"/>
     </row>
     <row r="59" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A59" s="29" t="s">
-        <v>195</v>
+        <v>257</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E59" s="59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F59" s="60"/>
       <c r="G59" s="60"/>
@@ -6332,37 +6383,37 @@
         <v>0</v>
       </c>
       <c r="J59" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K59" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L59" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N59" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O59" s="31"/>
     </row>
-    <row r="60" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="60" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A60" s="29" t="s">
-        <v>196</v>
+        <v>258</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="E60" s="59" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
       <c r="F60" s="60"/>
       <c r="G60" s="60"/>
@@ -6370,11 +6421,9 @@
         <v>42843</v>
       </c>
       <c r="I60" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J60" s="46" t="s">
-        <v>99</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J60" s="37"/>
       <c r="K60" s="54" t="s">
         <v>160</v>
       </c>
@@ -6382,67 +6431,47 @@
         <v>18</v>
       </c>
       <c r="M60" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N60" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O60" s="31"/>
     </row>
-    <row r="61" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
-      <c r="A61" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="B61" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="45">
-        <v>42843</v>
-      </c>
-      <c r="I61" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J61" s="46"/>
-      <c r="K61" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="L61" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M61" s="50" t="s">
-        <v>257</v>
-      </c>
-      <c r="N61" s="50" t="s">
-        <v>254</v>
-      </c>
-      <c r="O61" s="31"/>
-    </row>
-    <row r="62" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
+    <row r="61" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A61" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="B61" s="70"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="70"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="70"/>
+      <c r="G61" s="70"/>
+      <c r="H61" s="70"/>
+      <c r="I61" s="70"/>
+      <c r="J61" s="70"/>
+      <c r="K61" s="70"/>
+      <c r="L61" s="70"/>
+      <c r="M61" s="70"/>
+      <c r="N61" s="70"/>
+      <c r="O61" s="71"/>
+    </row>
+    <row r="62" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A62" s="29" t="s">
-        <v>199</v>
+        <v>255</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>110</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E62" s="59" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F62" s="60"/>
       <c r="G62" s="60"/>
@@ -6452,36 +6481,36 @@
       <c r="I62" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J62" s="37"/>
+      <c r="J62" s="46"/>
       <c r="K62" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L62" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N62" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O62" s="31"/>
     </row>
     <row r="63" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A63" s="29" t="s">
-        <v>198</v>
+        <v>254</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>155</v>
+        <v>94</v>
       </c>
       <c r="E63" s="59" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="F63" s="60"/>
       <c r="G63" s="60"/>
@@ -6489,96 +6518,98 @@
         <v>42843</v>
       </c>
       <c r="I63" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J63" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="46" t="s">
+        <v>98</v>
+      </c>
       <c r="K63" s="54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L63" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N63" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O63" s="31"/>
     </row>
-    <row r="64" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A64" s="69" t="s">
-        <v>205</v>
-      </c>
-      <c r="B64" s="70"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="70"/>
-      <c r="E64" s="70"/>
-      <c r="F64" s="70"/>
-      <c r="G64" s="70"/>
-      <c r="H64" s="70"/>
-      <c r="I64" s="70"/>
-      <c r="J64" s="70"/>
-      <c r="K64" s="70"/>
-      <c r="L64" s="70"/>
-      <c r="M64" s="70"/>
-      <c r="N64" s="70"/>
-      <c r="O64" s="71"/>
-    </row>
-    <row r="65" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
-      <c r="A65" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="B65" s="39" t="s">
+    <row r="64" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+      <c r="A64" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" s="59" t="s">
+        <v>151</v>
+      </c>
+      <c r="F64" s="60"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="45">
+        <v>42843</v>
+      </c>
+      <c r="I64" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="46"/>
+      <c r="K64" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="L64" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M64" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="N64" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="O64" s="31"/>
+    </row>
+    <row r="65" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A65" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="B65" s="70"/>
+      <c r="C65" s="70"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="70"/>
+      <c r="F65" s="70"/>
+      <c r="G65" s="70"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="70"/>
+      <c r="J65" s="70"/>
+      <c r="K65" s="70"/>
+      <c r="L65" s="70"/>
+      <c r="M65" s="70"/>
+      <c r="N65" s="70"/>
+      <c r="O65" s="71"/>
+    </row>
+    <row r="66" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="A66" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="D66" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="E66" s="59" t="s">
         <v>115</v>
-      </c>
-      <c r="E65" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="45">
-        <v>42847</v>
-      </c>
-      <c r="I65" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J65" s="46"/>
-      <c r="K65" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L65" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M65" s="50" t="s">
-        <v>257</v>
-      </c>
-      <c r="N65" s="50" t="s">
-        <v>254</v>
-      </c>
-      <c r="O65" s="31"/>
-    </row>
-    <row r="66" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
-      <c r="A66" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B66" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E66" s="59" t="s">
-        <v>156</v>
       </c>
       <c r="F66" s="60"/>
       <c r="G66" s="60"/>
@@ -6590,34 +6621,34 @@
       </c>
       <c r="J66" s="46"/>
       <c r="K66" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L66" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N66" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O66" s="31"/>
     </row>
-    <row r="67" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+    <row r="67" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A67" s="29" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B67" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D67" s="28" t="s">
-        <v>157</v>
-      </c>
       <c r="E67" s="59" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F67" s="60"/>
       <c r="G67" s="60"/>
@@ -6629,34 +6660,34 @@
       </c>
       <c r="J67" s="46"/>
       <c r="K67" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L67" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N67" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O67" s="31"/>
     </row>
     <row r="68" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A68" s="29" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="E68" s="59" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="F68" s="60"/>
       <c r="G68" s="60"/>
@@ -6664,40 +6695,38 @@
         <v>42847</v>
       </c>
       <c r="I68" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J68" s="46" t="s">
-        <v>125</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J68" s="46"/>
       <c r="K68" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L68" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N68" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O68" s="31"/>
     </row>
     <row r="69" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A69" s="29" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B69" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="31" t="s">
+      <c r="D69" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D69" s="28" t="s">
-        <v>123</v>
-      </c>
       <c r="E69" s="59" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F69" s="60"/>
       <c r="G69" s="60"/>
@@ -6705,33 +6734,63 @@
         <v>42847</v>
       </c>
       <c r="I69" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J69" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J69" s="46" t="s">
+        <v>124</v>
+      </c>
       <c r="K69" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L69" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="N69" s="50" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="O69" s="31"/>
     </row>
-    <row r="70" spans="1:15" ht="12" customHeight="1">
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="I70" s="55"/>
-      <c r="J70"/>
-      <c r="K70" s="55"/>
-      <c r="L70"/>
-      <c r="M70"/>
-      <c r="N70"/>
-      <c r="O70"/>
+    <row r="70" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+      <c r="A70" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="F70" s="60"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="45">
+        <v>42847</v>
+      </c>
+      <c r="I70" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" s="46"/>
+      <c r="K70" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L70" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M70" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="N70" s="50" t="s">
+        <v>241</v>
+      </c>
+      <c r="O70" s="31"/>
     </row>
     <row r="71" spans="1:15" ht="12" customHeight="1">
       <c r="B71"/>
@@ -6832,7 +6891,9 @@
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="1:15" ht="13.5">
+    <row r="80" spans="1:15" ht="12" customHeight="1">
+      <c r="B80"/>
+      <c r="C80"/>
       <c r="I80" s="55"/>
       <c r="J80"/>
       <c r="K80" s="55"/>
@@ -11098,24 +11159,34 @@
       <c r="N553"/>
       <c r="O553"/>
     </row>
+    <row r="554" spans="9:15" ht="13.5">
+      <c r="I554" s="55"/>
+      <c r="J554"/>
+      <c r="K554" s="55"/>
+      <c r="L554"/>
+      <c r="M554"/>
+      <c r="N554"/>
+      <c r="O554"/>
+    </row>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="E65:G65"/>
+  <mergeCells count="82">
     <mergeCell ref="E66:G66"/>
     <mergeCell ref="E67:G67"/>
     <mergeCell ref="E68:G68"/>
     <mergeCell ref="E69:G69"/>
-    <mergeCell ref="A64:O64"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="A65:O65"/>
+    <mergeCell ref="E60:G60"/>
     <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
     <mergeCell ref="E54:G54"/>
     <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E58:G58"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="E56:G56"/>
     <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A61:O61"/>
     <mergeCell ref="E49:G49"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="E51:G51"/>
@@ -11183,33 +11254,49 @@
     <mergeCell ref="E27:G27"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I1:I60 I62:I1048576">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Not">
+  <conditionalFormatting sqref="M1:M60 M62:M1048576">
+    <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="Not">
       <formula>LEFT(M1,LEN("Not"))="Not"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M53:M63 M38:M43 M13:M16 M18:M36 M45:M51 M65:M69">
+  <conditionalFormatting sqref="I61">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I61)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M61">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Not">
+      <formula>LEFT(M61,LEN("Not"))="Not"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",M61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M66:M70 M38:M43 M13:M16 M18:M36 M45:M51 M62:M64 M53:M57 M58:M60">
       <formula1>$S$1:$S$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N53:N63 N65:N69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N66:N70 N62:N64 N53:N57 N58:N60">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I54:I63 I65:I69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I66:I70 I62:I64 I54:I57 I58:I60">
       <formula1>$R$1:$R$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K53:K63 K65:K69">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K66:K70 K62:K64 K53:K57 K58:K60">
       <formula1>$Q$1:$Q$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added test cases for Edit Article
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="254">
   <si>
     <t>Fail</t>
   </si>
@@ -362,9 +362,6 @@
 4: Click on "Cancel" button</t>
   </si>
   <si>
-    <t>user should be redirected back to previously visited page</t>
-  </si>
-  <si>
     <t>Test if "Cancel" button is working properly with filled "Title" and "Content" fields</t>
   </si>
   <si>
@@ -439,14 +436,6 @@
   </si>
   <si>
     <t>"Delete" button exist, but user can't actualy delete the page</t>
-  </si>
-  <si>
-    <t>Test if "Back" button is working properly</t>
-  </si>
-  <si>
-    <t>1: Open blog "Home" page
-2: Click on any article
-3: Click on "Back" button</t>
   </si>
   <si>
     <t>1: Open blog "Home" page
@@ -468,9 +457,6 @@
     <t>1. Logged as Regular User 2. At least one exisiting article not created by currently logged user</t>
   </si>
   <si>
-    <t>1. Logged as Regular User 2. At least one exisiting article</t>
-  </si>
-  <si>
     <t>1. Logged as Regular User 2. At least one exisiting article created by the currently logged user</t>
   </si>
   <si>
@@ -580,13 +566,6 @@
     <t>1: Open blog "Home" page
 2: Click on any article created by currently logged user 3: Click on "Edit" button
 4: Type "Test Automation is the key" in "Title" field(any title with more that 5 characters and less than 50 characters).
-5: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field(any text with more that 100 characters and less than 10 000 characters).
-6: Click on "Edit" button</t>
-  </si>
-  <si>
-    <t>1: Open blog "Home" page
-2: Click on any article created by currently logged user 3: Click on "Edit" button
-4: Type "Test Automation is the key" in "Title" field(any title with more that 5 characters and less than 50 characters).
 5: Type "Traditional quality assurance..." in "Content" field(any text with less that 100 characters).
 6: Click on "Edit" button</t>
   </si>
@@ -611,13 +590,6 @@
     <t>Edit Own Article with title with more than 50 characters(including spaces)</t>
   </si>
   <si>
-    <t>1: Open blog "Home" page
-2: Click on any article created by currently logged user 3: Click on "Edit" button
-4: Type "Test Automation Process is the key" in "Title" field(any title with more 50 characters).
-5: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field(any text with more that 100 characters and less than 10 000 characters).
-6: Click on "Edit" button</t>
-  </si>
-  <si>
     <t>"Invalid login attempt." message should be shown to user</t>
   </si>
   <si>
@@ -1005,7 +977,18 @@
     <t>EAP_TC7</t>
   </si>
   <si>
-    <t>EAP_TC8</t>
+    <t>1: Open blog "Home" page
+2: Click on any article created by currently logged user 3: Click on "Edit" button
+4: Type "This article has been Edited" in "Title" field(any title with more that 5 characters and less than 50 characters).
+5: Type "This article has been Edited. The original content of the article was starting with: Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field(any text with more that 100 characters and less than 10 000 characters).
+6: Click on "Edit" button</t>
+  </si>
+  <si>
+    <t>1: Open blog "Home" page
+2: Click on any article created by currently logged user 3: Click on "Edit" button
+4: Type any content that contains more than 50 characters(including spaces) in "Title" field(any title with more 50 characters).
+5: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field(any text with more that 100 characters and less than 10 000 characters).
+6: Click on "Edit" button</t>
   </si>
 </sst>
 </file>
@@ -1576,23 +1559,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1612,15 +1625,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1632,9 +1636,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1648,55 +1649,13 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1_Vanco_CR022a1_TestCase_v0.1" xfId="1"/>
     <cellStyle name="標準_結合試験(AllOvertheWorld)" xfId="2"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -4342,12 +4301,12 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:T554"/>
+  <dimension ref="A1:T553"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="A60" sqref="A60"/>
+      <selection pane="topRight" activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4370,10 +4329,10 @@
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -4386,24 +4345,24 @@
       <c r="O1" s="43"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -4416,90 +4375,90 @@
       <c r="O2" s="43"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="25.5">
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
       <c r="P4" s="7"/>
       <c r="T4" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="23" customFormat="1" ht="25.5">
       <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="68"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="78"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
       <c r="P5" s="22"/>
       <c r="T5" s="23" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4507,27 +4466,27 @@
         <v>13</v>
       </c>
       <c r="B6" s="32">
-        <f>COUNTIF(I17:I138,"Pass")</f>
-        <v>34</v>
+        <f>COUNTIF(I17:I137,"Pass")</f>
+        <v>33</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="10">
-        <f>COUNTIF(I10:I761,"Pending")</f>
+        <f>COUNTIF(I10:I760,"Pending")</f>
         <v>0</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="N6" s="73"/>
-      <c r="O6" s="73"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -4535,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="33">
-        <f>COUNTIF(I17:I138,"Fail")</f>
+        <f>COUNTIF(I17:I137,"Fail")</f>
         <v>14</v>
       </c>
       <c r="C7" s="33"/>
@@ -4543,27 +4502,27 @@
         <v>6</v>
       </c>
       <c r="E7" s="15">
-        <f>COUNTIF(A17:A138,"TC*")</f>
+        <f>COUNTIF(A17:A137,"TC*")</f>
         <v>0</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="73"/>
-      <c r="O7" s="73"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -4577,119 +4536,119 @@
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:20" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="82" t="s">
+      <c r="E9" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="80" t="s">
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="62" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="L9" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="57" t="s">
-        <v>222</v>
-      </c>
-      <c r="N9" s="57" t="s">
-        <v>238</v>
-      </c>
-      <c r="O9" s="76" t="s">
+      <c r="M9" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="N9" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="O9" s="64" t="s">
         <v>10</v>
       </c>
       <c r="P9" s="24"/>
     </row>
     <row r="10" spans="1:20" s="19" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="58"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="63"/>
       <c r="K10" s="48"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="76"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="64"/>
       <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:20" s="26" customFormat="1" ht="15">
-      <c r="A11" s="85"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="86"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="72"/>
     </row>
     <row r="12" spans="1:20" s="3" customFormat="1" ht="12.75">
-      <c r="A12" s="69" t="s">
-        <v>204</v>
-      </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
-      <c r="N12" s="70"/>
-      <c r="O12" s="71"/>
+      <c r="A12" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="61"/>
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="76.5" customHeight="1" outlineLevel="1">
       <c r="A13" s="29" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>208</v>
-      </c>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
+        <v>201</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="45">
         <v>42841</v>
       </c>
@@ -4698,35 +4657,35 @@
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N13" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:20" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A14" s="29" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" s="61" t="s">
-        <v>211</v>
-      </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
+        <v>204</v>
+      </c>
+      <c r="E14" s="69" t="s">
+        <v>205</v>
+      </c>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
       <c r="H14" s="45">
         <v>42841</v>
       </c>
@@ -4735,33 +4694,33 @@
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L14" s="28"/>
       <c r="M14" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N14" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A15" s="29" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="E15" s="61" t="s">
-        <v>214</v>
-      </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
+        <v>207</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>208</v>
+      </c>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
       <c r="H15" s="45">
         <v>42841</v>
       </c>
@@ -4770,33 +4729,33 @@
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L15" s="28"/>
       <c r="M15" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N15" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A16" s="29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="E16" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
+        <v>210</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
       <c r="H16" s="45">
         <v>42841</v>
       </c>
@@ -4805,52 +4764,52 @@
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L16" s="28"/>
       <c r="M16" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N16" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O16" s="27"/>
     </row>
     <row r="17" spans="1:19" s="3" customFormat="1" ht="12.75">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="71"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="61"/>
     </row>
     <row r="18" spans="1:19" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A18" s="29" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>225</v>
-      </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
+        <v>218</v>
+      </c>
+      <c r="E18" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="45">
         <v>42841</v>
       </c>
@@ -4859,22 +4818,22 @@
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N18" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A19" s="29" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>15</v>
@@ -4883,11 +4842,11 @@
       <c r="D19" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
+      <c r="E19" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="45">
         <v>42841</v>
       </c>
@@ -4896,22 +4855,22 @@
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N19" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A20" s="29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>19</v>
@@ -4920,11 +4879,11 @@
       <c r="D20" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="45">
         <v>42841</v>
       </c>
@@ -4933,22 +4892,22 @@
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L20" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N20" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A21" s="29" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>21</v>
@@ -4957,11 +4916,11 @@
       <c r="D21" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="61" t="s">
+      <c r="E21" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="45">
         <v>42841</v>
       </c>
@@ -4972,22 +4931,22 @@
         <v>24</v>
       </c>
       <c r="K21" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L21" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N21" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:19" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A22" s="29" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B22" s="39" t="s">
         <v>25</v>
@@ -4996,11 +4955,11 @@
       <c r="D22" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
       <c r="H22" s="45">
         <v>42841</v>
       </c>
@@ -5009,22 +4968,22 @@
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L22" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N22" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O22" s="27"/>
     </row>
     <row r="23" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A23" s="29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>27</v>
@@ -5033,11 +4992,11 @@
       <c r="D23" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E23" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="45">
         <v>42841</v>
       </c>
@@ -5048,35 +5007,35 @@
         <v>30</v>
       </c>
       <c r="K23" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L23" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N23" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A24" s="29" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E24" s="59" t="s">
-        <v>194</v>
-      </c>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
+        <v>191</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
       <c r="H24" s="45">
         <v>42841</v>
       </c>
@@ -5085,22 +5044,22 @@
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N24" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B25" s="39" t="s">
         <v>34</v>
@@ -5109,11 +5068,11 @@
       <c r="D25" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="45">
         <v>42841</v>
       </c>
@@ -5124,22 +5083,22 @@
         <v>32</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L25" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N25" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B26" s="39" t="s">
         <v>33</v>
@@ -5148,11 +5107,11 @@
       <c r="D26" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
       <c r="H26" s="45">
         <v>42841</v>
       </c>
@@ -5161,22 +5120,22 @@
       </c>
       <c r="J26" s="28"/>
       <c r="K26" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L26" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N26" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A27" s="29" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>37</v>
@@ -5185,11 +5144,11 @@
       <c r="D27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="61" t="s">
+      <c r="E27" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="45">
         <v>42841</v>
       </c>
@@ -5198,22 +5157,22 @@
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L27" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A28" s="29" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B28" s="39" t="s">
         <v>40</v>
@@ -5222,11 +5181,11 @@
       <c r="D28" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
       <c r="H28" s="45">
         <v>42841</v>
       </c>
@@ -5237,35 +5196,35 @@
         <v>30</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L28" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O28" s="31"/>
     </row>
     <row r="29" spans="1:19" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A29" s="29" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
+        <v>192</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
       <c r="H29" s="45">
         <v>42841</v>
       </c>
@@ -5276,16 +5235,16 @@
         <v>32</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L29" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="40"/>
@@ -5295,7 +5254,7 @@
     </row>
     <row r="30" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A30" s="29" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B30" s="39" t="s">
         <v>43</v>
@@ -5304,11 +5263,11 @@
       <c r="D30" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="59" t="s">
+      <c r="E30" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
       <c r="H30" s="45">
         <v>42841</v>
       </c>
@@ -5317,22 +5276,22 @@
       </c>
       <c r="J30" s="37"/>
       <c r="K30" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L30" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N30" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O30" s="31"/>
     </row>
     <row r="31" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A31" s="29" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B31" s="39" t="s">
         <v>47</v>
@@ -5341,11 +5300,11 @@
       <c r="D31" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
       <c r="H31" s="45">
         <v>42841</v>
       </c>
@@ -5354,22 +5313,22 @@
       </c>
       <c r="J31" s="37"/>
       <c r="K31" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N31" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O31" s="31"/>
     </row>
     <row r="32" spans="1:19" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A32" s="29" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>51</v>
@@ -5378,11 +5337,11 @@
       <c r="D32" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
       <c r="H32" s="45">
         <v>42841</v>
       </c>
@@ -5391,22 +5350,22 @@
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L32" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N32" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O32" s="31"/>
     </row>
     <row r="33" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A33" s="29" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B33" s="39" t="s">
         <v>54</v>
@@ -5415,11 +5374,11 @@
       <c r="D33" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="59" t="s">
+      <c r="E33" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
       <c r="H33" s="45">
         <v>42841</v>
       </c>
@@ -5428,35 +5387,35 @@
       </c>
       <c r="J33" s="37"/>
       <c r="K33" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L33" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M33" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N33" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O33" s="31"/>
     </row>
     <row r="34" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A34" s="51" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C34" s="39"/>
       <c r="D34" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="E34" s="59" t="s">
-        <v>231</v>
-      </c>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
+        <v>224</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
       <c r="H34" s="45">
         <v>42841</v>
       </c>
@@ -5465,35 +5424,35 @@
       </c>
       <c r="J34" s="37"/>
       <c r="K34" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L34" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M34" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N34" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O34" s="31"/>
     </row>
     <row r="35" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A35" s="51" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C35" s="39"/>
       <c r="D35" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>234</v>
-      </c>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
+        <v>227</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>228</v>
+      </c>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="45">
         <v>42841</v>
       </c>
@@ -5502,35 +5461,35 @@
       </c>
       <c r="J35" s="37"/>
       <c r="K35" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L35" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M35" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N35" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O35" s="31"/>
     </row>
     <row r="36" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A36" s="51" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C36" s="39"/>
       <c r="D36" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="E36" s="59" t="s">
-        <v>237</v>
-      </c>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
+        <v>230</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="45">
         <v>42841</v>
       </c>
@@ -5539,56 +5498,56 @@
       </c>
       <c r="J36" s="37"/>
       <c r="K36" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L36" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M36" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O36" s="31"/>
     </row>
     <row r="37" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="71"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="61"/>
     </row>
     <row r="38" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A38" s="29" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="59" t="s">
+      <c r="E38" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="45">
         <v>42843</v>
       </c>
@@ -5597,22 +5556,22 @@
       </c>
       <c r="J38" s="37"/>
       <c r="K38" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L38" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M38" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N38" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O38" s="31"/>
     </row>
     <row r="39" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A39" s="29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>62</v>
@@ -5621,11 +5580,11 @@
       <c r="D39" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
       <c r="H39" s="45">
         <v>42843</v>
       </c>
@@ -5634,22 +5593,22 @@
       </c>
       <c r="J39" s="37"/>
       <c r="K39" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L39" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M39" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N39" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O39" s="31"/>
     </row>
     <row r="40" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A40" s="29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B40" s="39" t="s">
         <v>63</v>
@@ -5660,11 +5619,11 @@
       <c r="D40" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
+      <c r="E40" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
       <c r="H40" s="45">
         <v>42843</v>
       </c>
@@ -5673,22 +5632,22 @@
       </c>
       <c r="J40" s="37"/>
       <c r="K40" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L40" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M40" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O40" s="31"/>
     </row>
     <row r="41" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A41" s="29" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B41" s="39" t="s">
         <v>64</v>
@@ -5699,11 +5658,11 @@
       <c r="D41" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
+      <c r="E41" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
       <c r="H41" s="45">
         <v>42843</v>
       </c>
@@ -5712,35 +5671,35 @@
       </c>
       <c r="J41" s="37"/>
       <c r="K41" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L41" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M41" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O41" s="31"/>
     </row>
     <row r="42" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A42" s="29" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="E42" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
+        <v>196</v>
+      </c>
+      <c r="E42" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
       <c r="H42" s="45">
         <v>42869</v>
       </c>
@@ -5749,37 +5708,37 @@
       </c>
       <c r="J42" s="37"/>
       <c r="K42" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L42" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M42" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O42" s="31"/>
     </row>
     <row r="43" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A43" s="29" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
+        <v>123</v>
+      </c>
+      <c r="E43" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
       <c r="H43" s="45">
         <v>42843</v>
       </c>
@@ -5788,56 +5747,56 @@
       </c>
       <c r="J43" s="37"/>
       <c r="K43" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L43" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M43" s="52" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O43" s="31"/>
     </row>
     <row r="44" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A44" s="69" t="s">
+      <c r="A44" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="70"/>
-      <c r="K44" s="70"/>
-      <c r="L44" s="70"/>
-      <c r="M44" s="70"/>
-      <c r="N44" s="70"/>
-      <c r="O44" s="71"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="60"/>
+      <c r="K44" s="60"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="61"/>
     </row>
     <row r="45" spans="1:15" s="30" customFormat="1" ht="140.25" outlineLevel="1">
       <c r="A45" s="29" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B45" s="39" t="s">
         <v>68</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
+      <c r="E45" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
       <c r="H45" s="45">
         <v>42843</v>
       </c>
@@ -5846,37 +5805,37 @@
       </c>
       <c r="J45" s="37"/>
       <c r="K45" s="54" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L45" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M45" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N45" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O45" s="31"/>
     </row>
     <row r="46" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A46" s="29" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B46" s="39" t="s">
         <v>76</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
+      <c r="E46" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
       <c r="H46" s="45">
         <v>42843</v>
       </c>
@@ -5885,37 +5844,37 @@
       </c>
       <c r="J46" s="37"/>
       <c r="K46" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L46" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M46" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O46" s="31"/>
     </row>
     <row r="47" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A47" s="29" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B47" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D47" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
+      <c r="E47" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
       <c r="H47" s="45">
         <v>42843</v>
       </c>
@@ -5924,37 +5883,37 @@
       </c>
       <c r="J47" s="37"/>
       <c r="K47" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L47" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M47" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O47" s="31"/>
     </row>
     <row r="48" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A48" s="29" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="59" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" s="60"/>
-      <c r="G48" s="60"/>
+        <v>80</v>
+      </c>
+      <c r="E48" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
       <c r="H48" s="45">
         <v>42843</v>
       </c>
@@ -5962,40 +5921,40 @@
         <v>0</v>
       </c>
       <c r="J48" s="46" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="K48" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L48" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M48" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O48" s="31"/>
     </row>
     <row r="49" spans="1:15" s="30" customFormat="1" ht="102" outlineLevel="1">
       <c r="A49" s="29" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E49" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="F49" s="60"/>
-      <c r="G49" s="60"/>
+        <v>132</v>
+      </c>
+      <c r="E49" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
       <c r="H49" s="45">
         <v>42843</v>
       </c>
@@ -6004,37 +5963,37 @@
       </c>
       <c r="J49" s="46"/>
       <c r="K49" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L49" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M49" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N49" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O49" s="31"/>
     </row>
     <row r="50" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A50" s="29" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+        <v>81</v>
+      </c>
+      <c r="E50" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
       <c r="H50" s="45">
         <v>42843</v>
       </c>
@@ -6042,40 +6001,40 @@
         <v>0</v>
       </c>
       <c r="J50" s="46" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="K50" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L50" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="50" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N50" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O50" s="31"/>
     </row>
     <row r="51" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A51" s="29" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B51" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E51" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
+      <c r="E51" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="45">
         <v>42843</v>
       </c>
@@ -6083,59 +6042,59 @@
         <v>0</v>
       </c>
       <c r="J51" s="46" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K51" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L51" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M51" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N51" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A52" s="69" t="s">
-        <v>246</v>
-      </c>
-      <c r="B52" s="70"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
-      <c r="I52" s="70"/>
-      <c r="J52" s="70"/>
-      <c r="K52" s="70"/>
-      <c r="L52" s="70"/>
-      <c r="M52" s="70"/>
-      <c r="N52" s="70"/>
-      <c r="O52" s="71"/>
-    </row>
-    <row r="53" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
+      <c r="A52" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="60"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="60"/>
+      <c r="M52" s="60"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="61"/>
+    </row>
+    <row r="53" spans="1:15" s="30" customFormat="1" ht="178.5" outlineLevel="1">
       <c r="A53" s="29" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E53" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
+        <v>252</v>
+      </c>
+      <c r="E53" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
       <c r="H53" s="45">
         <v>42843</v>
       </c>
@@ -6144,37 +6103,37 @@
       </c>
       <c r="J53" s="37"/>
       <c r="K53" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L53" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M53" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N53" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O53" s="31"/>
     </row>
     <row r="54" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A54" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E54" s="59" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="60"/>
-      <c r="G54" s="60"/>
+        <v>98</v>
+      </c>
+      <c r="E54" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="45">
         <v>42843</v>
       </c>
@@ -6182,40 +6141,40 @@
         <v>0</v>
       </c>
       <c r="J54" s="46" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K54" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L54" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M54" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="N54" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="O54" s="31"/>
+    </row>
+    <row r="55" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
+      <c r="A55" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="N54" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="O54" s="31"/>
-    </row>
-    <row r="55" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
-      <c r="A55" s="29" t="s">
-        <v>250</v>
-      </c>
       <c r="B55" s="39" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E55" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
+        <v>253</v>
+      </c>
+      <c r="E55" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
       <c r="H55" s="45">
         <v>42843</v>
       </c>
@@ -6224,37 +6183,37 @@
       </c>
       <c r="J55" s="37"/>
       <c r="K55" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L55" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N55" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O55" s="31"/>
     </row>
     <row r="56" spans="1:15" s="30" customFormat="1" ht="127.5" outlineLevel="1">
       <c r="A56" s="29" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B56" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="31" t="s">
-        <v>107</v>
-      </c>
       <c r="D56" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E56" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="60"/>
-      <c r="G56" s="60"/>
+        <v>133</v>
+      </c>
+      <c r="E56" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
       <c r="H56" s="45">
         <v>42843</v>
       </c>
@@ -6262,40 +6221,40 @@
         <v>0</v>
       </c>
       <c r="J56" s="46" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K56" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L56" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N56" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O56" s="31"/>
     </row>
     <row r="57" spans="1:15" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A57" s="29" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D57" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
       <c r="H57" s="45">
         <v>42843</v>
       </c>
@@ -6303,301 +6262,301 @@
         <v>0</v>
       </c>
       <c r="J57" s="46" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K57" s="54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L57" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N57" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O57" s="31"/>
     </row>
-    <row r="58" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
+    <row r="58" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A58" s="29" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E58" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" s="60"/>
-      <c r="G58" s="60"/>
+        <v>94</v>
+      </c>
+      <c r="E58" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
       <c r="H58" s="45">
         <v>42843</v>
       </c>
       <c r="I58" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J58" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="46" t="s">
+        <v>90</v>
+      </c>
       <c r="K58" s="54" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L58" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N58" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O58" s="31"/>
     </row>
-    <row r="59" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="59" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A59" s="29" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C59" s="31" t="s">
         <v>105</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E59" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+        <v>135</v>
+      </c>
+      <c r="E59" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F59" s="58"/>
+      <c r="G59" s="58"/>
       <c r="H59" s="45">
         <v>42843</v>
       </c>
       <c r="I59" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J59" s="46" t="s">
-        <v>91</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J59" s="37"/>
       <c r="K59" s="54" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L59" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N59" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="O59" s="31"/>
+    </row>
+    <row r="60" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A60" s="59" t="s">
         <v>241</v>
       </c>
-      <c r="O59" s="31"/>
-    </row>
-    <row r="60" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
-      <c r="A60" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="B60" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D60" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="E60" s="59" t="s">
-        <v>153</v>
-      </c>
+      <c r="B60" s="60"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="60"/>
       <c r="G60" s="60"/>
-      <c r="H60" s="45">
+      <c r="H60" s="60"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="60"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="60"/>
+      <c r="N60" s="60"/>
+      <c r="O60" s="61"/>
+    </row>
+    <row r="61" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
+      <c r="A61" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B61" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E61" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="45">
         <v>42843</v>
       </c>
-      <c r="I60" s="54" t="s">
+      <c r="I61" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J60" s="37"/>
-      <c r="K60" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L60" s="28" t="s">
+      <c r="J61" s="46"/>
+      <c r="K61" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="L61" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M60" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="N60" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="O60" s="31"/>
-    </row>
-    <row r="61" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A61" s="69" t="s">
-        <v>247</v>
-      </c>
-      <c r="B61" s="70"/>
-      <c r="C61" s="70"/>
-      <c r="D61" s="70"/>
-      <c r="E61" s="70"/>
-      <c r="F61" s="70"/>
-      <c r="G61" s="70"/>
-      <c r="H61" s="70"/>
-      <c r="I61" s="70"/>
-      <c r="J61" s="70"/>
-      <c r="K61" s="70"/>
-      <c r="L61" s="70"/>
-      <c r="M61" s="70"/>
-      <c r="N61" s="70"/>
-      <c r="O61" s="71"/>
+      <c r="M61" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="N61" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="O61" s="31"/>
     </row>
     <row r="62" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A62" s="29" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E62" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="F62" s="60"/>
-      <c r="G62" s="60"/>
+        <v>93</v>
+      </c>
+      <c r="E62" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" s="58"/>
+      <c r="G62" s="58"/>
       <c r="H62" s="45">
         <v>42843</v>
       </c>
       <c r="I62" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J62" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="46" t="s">
+        <v>97</v>
+      </c>
       <c r="K62" s="54" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L62" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N62" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O62" s="31"/>
     </row>
     <row r="63" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A63" s="29" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>105</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E63" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="60"/>
-      <c r="G63" s="60"/>
+        <v>148</v>
+      </c>
+      <c r="E63" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="F63" s="58"/>
+      <c r="G63" s="58"/>
       <c r="H63" s="45">
         <v>42843</v>
       </c>
       <c r="I63" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J63" s="46" t="s">
-        <v>98</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J63" s="46"/>
       <c r="K63" s="54" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="L63" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N63" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O63" s="31"/>
     </row>
-    <row r="64" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A64" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="B64" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C64" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D64" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E64" s="59" t="s">
-        <v>151</v>
-      </c>
+    <row r="64" spans="1:15" s="3" customFormat="1" ht="12.75">
+      <c r="A64" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="B64" s="60"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="60"/>
       <c r="G64" s="60"/>
-      <c r="H64" s="45">
-        <v>42843</v>
-      </c>
-      <c r="I64" s="54" t="s">
+      <c r="H64" s="60"/>
+      <c r="I64" s="60"/>
+      <c r="J64" s="60"/>
+      <c r="K64" s="60"/>
+      <c r="L64" s="60"/>
+      <c r="M64" s="60"/>
+      <c r="N64" s="60"/>
+      <c r="O64" s="61"/>
+    </row>
+    <row r="65" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="A65" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E65" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="F65" s="58"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="45">
+        <v>42847</v>
+      </c>
+      <c r="I65" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="J64" s="46"/>
-      <c r="K64" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="L64" s="28" t="s">
+      <c r="J65" s="46"/>
+      <c r="K65" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="L65" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M64" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="N64" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="O64" s="31"/>
-    </row>
-    <row r="65" spans="1:15" s="3" customFormat="1" ht="12.75">
-      <c r="A65" s="69" t="s">
-        <v>248</v>
-      </c>
-      <c r="B65" s="70"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="70"/>
-      <c r="F65" s="70"/>
-      <c r="G65" s="70"/>
-      <c r="H65" s="70"/>
-      <c r="I65" s="70"/>
-      <c r="J65" s="70"/>
-      <c r="K65" s="70"/>
-      <c r="L65" s="70"/>
-      <c r="M65" s="70"/>
-      <c r="N65" s="70"/>
-      <c r="O65" s="71"/>
-    </row>
-    <row r="66" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
+      <c r="M65" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="N65" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="O65" s="31"/>
+    </row>
+    <row r="66" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A66" s="29" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B66" s="39" t="s">
         <v>112</v>
@@ -6606,13 +6565,13 @@
         <v>113</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E66" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
+      <c r="E66" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="F66" s="58"/>
+      <c r="G66" s="58"/>
       <c r="H66" s="45">
         <v>42847</v>
       </c>
@@ -6621,37 +6580,37 @@
       </c>
       <c r="J66" s="46"/>
       <c r="K66" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L66" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N66" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O66" s="31"/>
     </row>
-    <row r="67" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="67" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A67" s="29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="E67" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
+        <v>150</v>
+      </c>
+      <c r="E67" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="F67" s="58"/>
+      <c r="G67" s="58"/>
       <c r="H67" s="45">
         <v>42847</v>
       </c>
@@ -6660,137 +6619,109 @@
       </c>
       <c r="J67" s="46"/>
       <c r="K67" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L67" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N67" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O67" s="31"/>
     </row>
     <row r="68" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A68" s="29" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C68" s="31" t="s">
         <v>117</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="E68" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="F68" s="60"/>
-      <c r="G68" s="60"/>
+        <v>118</v>
+      </c>
+      <c r="E68" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F68" s="58"/>
+      <c r="G68" s="58"/>
       <c r="H68" s="45">
         <v>42847</v>
       </c>
       <c r="I68" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J68" s="46"/>
+        <v>0</v>
+      </c>
+      <c r="J68" s="46" t="s">
+        <v>120</v>
+      </c>
       <c r="K68" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L68" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N68" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O68" s="31"/>
     </row>
     <row r="69" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A69" s="29" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E69" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="F69" s="60"/>
-      <c r="G69" s="60"/>
+        <v>118</v>
+      </c>
+      <c r="E69" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
       <c r="H69" s="45">
         <v>42847</v>
       </c>
       <c r="I69" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J69" s="46" t="s">
-        <v>124</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J69" s="46"/>
       <c r="K69" s="54" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L69" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="N69" s="50" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O69" s="31"/>
     </row>
-    <row r="70" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
-      <c r="A70" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="B70" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D70" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E70" s="59" t="s">
-        <v>123</v>
-      </c>
-      <c r="F70" s="60"/>
-      <c r="G70" s="60"/>
-      <c r="H70" s="45">
-        <v>42847</v>
-      </c>
-      <c r="I70" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="J70" s="46"/>
-      <c r="K70" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="L70" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="M70" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="N70" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="O70" s="31"/>
+    <row r="70" spans="1:15" ht="12" customHeight="1">
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="I70" s="55"/>
+      <c r="J70"/>
+      <c r="K70" s="55"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
     </row>
     <row r="71" spans="1:15" ht="12" customHeight="1">
       <c r="B71"/>
@@ -6891,9 +6822,7 @@
       <c r="N79"/>
       <c r="O79"/>
     </row>
-    <row r="80" spans="1:15" ht="12" customHeight="1">
-      <c r="B80"/>
-      <c r="C80"/>
+    <row r="80" spans="1:15" ht="13.5">
       <c r="I80" s="55"/>
       <c r="J80"/>
       <c r="K80" s="55"/>
@@ -11159,44 +11088,47 @@
       <c r="N553"/>
       <c r="O553"/>
     </row>
-    <row r="554" spans="9:15" ht="13.5">
-      <c r="I554" s="55"/>
-      <c r="J554"/>
-      <c r="K554" s="55"/>
-      <c r="L554"/>
-      <c r="M554"/>
-      <c r="N554"/>
-      <c r="O554"/>
-    </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="A65:O65"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A61:O61"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="A52:O52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="A44:O44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+  <mergeCells count="81">
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A17:O17"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="A37:O37"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="J9:J10"/>
     <mergeCell ref="E40:G40"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="C9:C10"/>
@@ -11213,48 +11145,35 @@
     <mergeCell ref="A11:O11"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="A37:O37"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A17:O17"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="H7:O7"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="A44:O44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="A52:O52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="A64:O64"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A60:O60"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I60 I62:I1048576">
+  <conditionalFormatting sqref="I61:I1048576 I1:I59">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I1)))</formula>
     </cfRule>
@@ -11262,7 +11181,7 @@
       <formula>NOT(ISERROR(SEARCH("Pass",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M60 M62:M1048576">
+  <conditionalFormatting sqref="M61:M1048576 M1:M59">
     <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="Not">
       <formula>LEFT(M1,LEN("Not"))="Not"</formula>
     </cfRule>
@@ -11270,33 +11189,33 @@
       <formula>NOT(ISERROR(SEARCH("Automated",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I61">
+  <conditionalFormatting sqref="I60">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Fail",I60)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pass",I60)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M61">
+  <conditionalFormatting sqref="M60">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Not">
-      <formula>LEFT(M61,LEN("Not"))="Not"</formula>
+      <formula>LEFT(M60,LEN("Not"))="Not"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",M61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Automated",M60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M66:M70 M38:M43 M13:M16 M18:M36 M45:M51 M62:M64 M53:M57 M58:M60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M65:M69 M38:M43 M13:M16 M18:M36 M45:M51 M61:M63 M53:M59">
       <formula1>$S$1:$S$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N66:N70 N62:N64 N53:N57 N58:N60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N65:N69 N61:N63 N53:N59">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I66:I70 I62:I64 I54:I57 I58:I60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I65:I69 I61:I63 I54:I59">
       <formula1>$R$1:$R$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K66:K70 K62:K64 K53:K57 K58:K60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K65:K69 K61:K63 K53:K59">
       <formula1>$Q$1:$Q$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Exel TS description updated
TEst described
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftUni\Team Papaya\QA-Automation-Team-Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20250" windowHeight="7455" tabRatio="821"/>
   </bookViews>
@@ -29,12 +24,12 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="258">
   <si>
     <t>Fail</t>
   </si>
@@ -362,42 +357,6 @@
 4: Click on "Cancel" button</t>
   </si>
   <si>
-    <t>Test if "Cancel" button is working properly with filled "Title" and "Content" fields</t>
-  </si>
-  <si>
-    <t>1: Open blog "Create" page
-2: Type "Test Automation is the key" in "Title" field.
-3: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field.
-4: Click on "Cancel" button</t>
-  </si>
-  <si>
-    <t>1: Open blog "Create" page
-2: Type "Test" in "Title" field.
-3: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field.
-4: Click on "Create" button</t>
-  </si>
-  <si>
-    <t>1: Open blog "Create" page
-2: Type " Test Title" in "Title" field.
-3: Type "Traditional quality assurance has become..." in "Content" field.
-4: Click on "Create" button</t>
-  </si>
-  <si>
-    <t>Create article with title with less than 5 characters(including spaces)</t>
-  </si>
-  <si>
-    <t>Create article with title with less than 100 characters(including spaces)</t>
-  </si>
-  <si>
-    <t>Create article with title with more than 10 000 characters(including spaces)</t>
-  </si>
-  <si>
-    <t>1: Open blog "Create" page
-2: Type " Test Title" in "Title" field.
-3: Type any text with more than 10 000 characters(including spaces) in "Content" field.
-4: Click on "Create" button</t>
-  </si>
-  <si>
     <t>Edit Article with valid data</t>
   </si>
   <si>
@@ -557,12 +516,6 @@
 4: Click on "Create" button</t>
   </si>
   <si>
-    <t>1: Open blog "Create" page
-2: Type more than 50 characters(with spaces) in "Title" field.
-3: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field.
-4: Click on "Create" button</t>
-  </si>
-  <si>
     <t>1: Open blog "Home" page
 2: Click on any article created by currently logged user 3: Click on "Edit" button
 4: Type "Test Automation is the key" in "Title" field(any title with more that 5 characters and less than 50 characters).
@@ -584,9 +537,6 @@
 6: Click on "Edit" button</t>
   </si>
   <si>
-    <t>Create article with title with more than 50 characters(including spaces)</t>
-  </si>
-  <si>
     <t>Edit Own Article with title with more than 50 characters(including spaces)</t>
   </si>
   <si>
@@ -606,9 +556,6 @@
   </si>
   <si>
     <t>Arcitcle is updated. Minimum characters required are 1</t>
-  </si>
-  <si>
-    <t>Arcitcle is created. Minimum characters required are 1</t>
   </si>
   <si>
     <t>Article is deleted. User is redirected to "Home"page</t>
@@ -989,6 +936,67 @@
 4: Type any content that contains more than 50 characters(including spaces) in "Title" field(any title with more 50 characters).
 5: Type "Traditional quality assurance has become a bottleneck in the development process and the advancement of test automation. Innovative development teams ..." in "Content" field(any text with more that 100 characters and less than 10 000 characters).
 6: Click on "Edit" button</t>
+  </si>
+  <si>
+    <t>Test Create Article Without Content</t>
+  </si>
+  <si>
+    <t>Create article without title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Open blog "Create" page
+2: Clear Title Field and type "Tralala" in the field
+3: Clear content field
+4: Click on "Create Article  Button" 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assert "The Content field is required."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Open blog "Create" page
+2: Clear title field
+3: Clear content field and type in content field "Tralala"
+4: Click on "Create" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assert "The Title field is required"</t>
+  </si>
+  <si>
+    <t>Create Article without content and without title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Open blog "Create" page
+2:Clear Title Field
+3: Clear Content field
+4: Clicl on Create button
+</t>
+  </si>
+  <si>
+    <t>Assert
+The Title field is required.", "The Content field is required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Open blog "Create" page
+</t>
+  </si>
+  <si>
+    <t>Assert element 
+Assert element text "Create Article"</t>
+  </si>
+  <si>
+    <t>Check create article page  displayed</t>
+  </si>
+  <si>
+    <t>Create Article Content Resize</t>
+  </si>
+  <si>
+    <t>1: Open blog "Create" page
+2: Resize content field</t>
+  </si>
+  <si>
+    <t>Assert content field size</t>
   </si>
 </sst>
 </file>
@@ -4054,7 +4062,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4089,7 +4097,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4303,10 +4311,10 @@
   </sheetPr>
   <dimension ref="A1:T553"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="A58" sqref="A58:XFD58"/>
+      <selection pane="topRight" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -4345,16 +4353,16 @@
       <c r="O1" s="43"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1">
@@ -4375,16 +4383,16 @@
       <c r="O2" s="43"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4409,10 +4417,10 @@
       <c r="O3" s="80"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="2" customFormat="1" ht="25.5">
@@ -4435,7 +4443,7 @@
       <c r="O4" s="80"/>
       <c r="P4" s="7"/>
       <c r="T4" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="23" customFormat="1" ht="25.5">
@@ -4458,7 +4466,7 @@
       <c r="O5" s="79"/>
       <c r="P5" s="22"/>
       <c r="T5" s="23" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1">
@@ -4467,7 +4475,7 @@
       </c>
       <c r="B6" s="32">
         <f>COUNTIF(I17:I137,"Pass")</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="8" t="s">
@@ -4495,7 +4503,7 @@
       </c>
       <c r="B7" s="33">
         <f>COUNTIF(I17:I137,"Fail")</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="12" t="s">
@@ -4563,16 +4571,16 @@
         <v>16</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="L9" s="62" t="s">
         <v>17</v>
       </c>
       <c r="M9" s="62" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="N9" s="62" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="O9" s="64" t="s">
         <v>10</v>
@@ -4616,7 +4624,7 @@
     </row>
     <row r="12" spans="1:20" s="3" customFormat="1" ht="12.75">
       <c r="A12" s="59" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
@@ -4635,17 +4643,17 @@
     </row>
     <row r="13" spans="1:20" s="3" customFormat="1" ht="76.5" customHeight="1" outlineLevel="1">
       <c r="A13" s="29" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="28" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E13" s="69" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
@@ -4657,32 +4665,32 @@
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L13" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N13" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O13" s="27"/>
     </row>
     <row r="14" spans="1:20" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A14" s="29" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="28" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="F14" s="70"/>
       <c r="G14" s="70"/>
@@ -4694,30 +4702,30 @@
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L14" s="28"/>
       <c r="M14" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N14" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O14" s="27"/>
     </row>
     <row r="15" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A15" s="29" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="28" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="E15" s="69" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F15" s="70"/>
       <c r="G15" s="70"/>
@@ -4729,30 +4737,30 @@
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L15" s="28"/>
       <c r="M15" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N15" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O15" s="27"/>
     </row>
     <row r="16" spans="1:20" s="3" customFormat="1" ht="38.25" outlineLevel="1">
       <c r="A16" s="29" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="28" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E16" s="69" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="F16" s="70"/>
       <c r="G16" s="70"/>
@@ -4764,14 +4772,14 @@
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L16" s="28"/>
       <c r="M16" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N16" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O16" s="27"/>
     </row>
@@ -4796,17 +4804,17 @@
     </row>
     <row r="18" spans="1:19" s="3" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A18" s="29" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="28" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="E18" s="69" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="F18" s="70"/>
       <c r="G18" s="70"/>
@@ -4818,22 +4826,22 @@
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M18" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N18" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O18" s="27"/>
     </row>
     <row r="19" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A19" s="29" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>15</v>
@@ -4843,7 +4851,7 @@
         <v>58</v>
       </c>
       <c r="E19" s="69" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F19" s="70"/>
       <c r="G19" s="70"/>
@@ -4855,22 +4863,22 @@
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M19" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N19" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O19" s="27"/>
     </row>
     <row r="20" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A20" s="29" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>19</v>
@@ -4892,22 +4900,22 @@
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L20" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M20" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N20" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O20" s="27"/>
     </row>
     <row r="21" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A21" s="29" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>21</v>
@@ -4931,22 +4939,22 @@
         <v>24</v>
       </c>
       <c r="K21" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L21" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N21" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O21" s="27"/>
     </row>
     <row r="22" spans="1:19" s="3" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A22" s="29" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B22" s="39" t="s">
         <v>25</v>
@@ -4968,22 +4976,22 @@
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L22" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N22" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O22" s="27"/>
     </row>
     <row r="23" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A23" s="29" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>27</v>
@@ -5007,32 +5015,32 @@
         <v>30</v>
       </c>
       <c r="K23" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L23" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N23" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A24" s="29" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C24" s="39"/>
       <c r="D24" s="28" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F24" s="58"/>
       <c r="G24" s="58"/>
@@ -5044,22 +5052,22 @@
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M24" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N24" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O24" s="27"/>
     </row>
     <row r="25" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A25" s="29" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B25" s="39" t="s">
         <v>34</v>
@@ -5083,22 +5091,22 @@
         <v>32</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L25" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N25" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O25" s="27"/>
     </row>
     <row r="26" spans="1:19" s="3" customFormat="1" ht="63.75" customHeight="1" outlineLevel="1">
       <c r="A26" s="29" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B26" s="39" t="s">
         <v>33</v>
@@ -5120,22 +5128,22 @@
       </c>
       <c r="J26" s="28"/>
       <c r="K26" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L26" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M26" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N26" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O26" s="27"/>
     </row>
     <row r="27" spans="1:19" s="3" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A27" s="29" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B27" s="39" t="s">
         <v>37</v>
@@ -5157,22 +5165,22 @@
       </c>
       <c r="J27" s="28"/>
       <c r="K27" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L27" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O27" s="27"/>
     </row>
     <row r="28" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A28" s="29" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B28" s="39" t="s">
         <v>40</v>
@@ -5196,32 +5204,32 @@
         <v>30</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L28" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M28" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N28" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O28" s="31"/>
     </row>
     <row r="29" spans="1:19" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A29" s="29" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="28" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F29" s="58"/>
       <c r="G29" s="58"/>
@@ -5235,16 +5243,16 @@
         <v>32</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L29" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O29" s="41"/>
       <c r="P29" s="40"/>
@@ -5254,7 +5262,7 @@
     </row>
     <row r="30" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A30" s="29" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B30" s="39" t="s">
         <v>43</v>
@@ -5276,22 +5284,22 @@
       </c>
       <c r="J30" s="37"/>
       <c r="K30" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L30" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M30" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N30" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O30" s="31"/>
     </row>
     <row r="31" spans="1:19" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A31" s="29" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B31" s="39" t="s">
         <v>47</v>
@@ -5313,22 +5321,22 @@
       </c>
       <c r="J31" s="37"/>
       <c r="K31" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M31" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N31" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O31" s="31"/>
     </row>
     <row r="32" spans="1:19" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A32" s="29" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B32" s="39" t="s">
         <v>51</v>
@@ -5350,22 +5358,22 @@
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L32" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M32" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N32" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O32" s="31"/>
     </row>
     <row r="33" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A33" s="29" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B33" s="39" t="s">
         <v>54</v>
@@ -5387,32 +5395,32 @@
       </c>
       <c r="J33" s="37"/>
       <c r="K33" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L33" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M33" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N33" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O33" s="31"/>
     </row>
     <row r="34" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A34" s="51" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C34" s="39"/>
       <c r="D34" s="28" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="F34" s="58"/>
       <c r="G34" s="58"/>
@@ -5424,32 +5432,32 @@
       </c>
       <c r="J34" s="37"/>
       <c r="K34" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L34" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M34" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N34" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O34" s="31"/>
     </row>
     <row r="35" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A35" s="51" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C35" s="39"/>
       <c r="D35" s="28" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="E35" s="57" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="F35" s="58"/>
       <c r="G35" s="58"/>
@@ -5461,32 +5469,32 @@
       </c>
       <c r="J35" s="37"/>
       <c r="K35" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L35" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M35" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N35" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O35" s="31"/>
     </row>
     <row r="36" spans="1:15" s="30" customFormat="1" ht="87.75" customHeight="1" outlineLevel="1">
       <c r="A36" s="51" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C36" s="39"/>
       <c r="D36" s="28" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="E36" s="57" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="F36" s="58"/>
       <c r="G36" s="58"/>
@@ -5498,16 +5506,16 @@
       </c>
       <c r="J36" s="37"/>
       <c r="K36" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L36" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M36" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N36" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O36" s="31"/>
     </row>
@@ -5532,13 +5540,13 @@
     </row>
     <row r="38" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A38" s="29" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>60</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>69</v>
@@ -5556,22 +5564,22 @@
       </c>
       <c r="J38" s="37"/>
       <c r="K38" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L38" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M38" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N38" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O38" s="31"/>
     </row>
     <row r="39" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A39" s="29" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>62</v>
@@ -5593,22 +5601,22 @@
       </c>
       <c r="J39" s="37"/>
       <c r="K39" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L39" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M39" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N39" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O39" s="31"/>
     </row>
     <row r="40" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A40" s="29" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B40" s="39" t="s">
         <v>63</v>
@@ -5620,7 +5628,7 @@
         <v>71</v>
       </c>
       <c r="E40" s="57" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F40" s="58"/>
       <c r="G40" s="58"/>
@@ -5632,22 +5640,22 @@
       </c>
       <c r="J40" s="37"/>
       <c r="K40" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L40" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M40" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N40" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O40" s="31"/>
     </row>
     <row r="41" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A41" s="29" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B41" s="39" t="s">
         <v>64</v>
@@ -5659,7 +5667,7 @@
         <v>72</v>
       </c>
       <c r="E41" s="57" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F41" s="58"/>
       <c r="G41" s="58"/>
@@ -5671,32 +5679,32 @@
       </c>
       <c r="J41" s="37"/>
       <c r="K41" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L41" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M41" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N41" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O41" s="31"/>
     </row>
     <row r="42" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A42" s="29" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="28" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="E42" s="57" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="F42" s="58"/>
       <c r="G42" s="58"/>
@@ -5708,34 +5716,34 @@
       </c>
       <c r="J42" s="37"/>
       <c r="K42" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L42" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M42" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N42" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O42" s="31"/>
     </row>
     <row r="43" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A43" s="29" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E43" s="57" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F43" s="58"/>
       <c r="G43" s="58"/>
@@ -5747,16 +5755,16 @@
       </c>
       <c r="J43" s="37"/>
       <c r="K43" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L43" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M43" s="52" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N43" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O43" s="31"/>
     </row>
@@ -5781,19 +5789,19 @@
     </row>
     <row r="45" spans="1:15" s="30" customFormat="1" ht="140.25" outlineLevel="1">
       <c r="A45" s="29" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B45" s="39" t="s">
         <v>68</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E45" s="57" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F45" s="58"/>
       <c r="G45" s="58"/>
@@ -5805,34 +5813,34 @@
       </c>
       <c r="J45" s="37"/>
       <c r="K45" s="54" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L45" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M45" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N45" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O45" s="31"/>
     </row>
     <row r="46" spans="1:15" s="30" customFormat="1" ht="51" outlineLevel="1">
       <c r="A46" s="29" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B46" s="39" t="s">
         <v>76</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="57" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F46" s="58"/>
       <c r="G46" s="58"/>
@@ -5844,34 +5852,34 @@
       </c>
       <c r="J46" s="37"/>
       <c r="K46" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L46" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M46" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N46" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O46" s="31"/>
     </row>
-    <row r="47" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="47" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A47" s="29" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>78</v>
+        <v>243</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>79</v>
+        <v>245</v>
       </c>
       <c r="E47" s="57" t="s">
-        <v>128</v>
+        <v>246</v>
       </c>
       <c r="F47" s="58"/>
       <c r="G47" s="58"/>
@@ -5883,34 +5891,34 @@
       </c>
       <c r="J47" s="37"/>
       <c r="K47" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L47" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M47" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N47" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O47" s="31"/>
     </row>
-    <row r="48" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
+    <row r="48" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A48" s="29" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>82</v>
+        <v>244</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>80</v>
+        <v>247</v>
       </c>
       <c r="E48" s="57" t="s">
-        <v>129</v>
+        <v>248</v>
       </c>
       <c r="F48" s="58"/>
       <c r="G48" s="58"/>
@@ -5918,40 +5926,38 @@
         <v>42843</v>
       </c>
       <c r="I48" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J48" s="46" t="s">
-        <v>144</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J48" s="46"/>
       <c r="K48" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L48" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M48" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N48" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O48" s="31"/>
     </row>
-    <row r="49" spans="1:15" s="30" customFormat="1" ht="102" outlineLevel="1">
+    <row r="49" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A49" s="29" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>136</v>
+        <v>249</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="E49" s="57" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="F49" s="58"/>
       <c r="G49" s="58"/>
@@ -5963,34 +5969,34 @@
       </c>
       <c r="J49" s="46"/>
       <c r="K49" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L49" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M49" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N49" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O49" s="31"/>
     </row>
-    <row r="50" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="50" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A50" s="29" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>83</v>
+        <v>254</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>81</v>
+        <v>252</v>
       </c>
       <c r="E50" s="57" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
       <c r="F50" s="58"/>
       <c r="G50" s="58"/>
@@ -5998,40 +6004,38 @@
         <v>42843</v>
       </c>
       <c r="I50" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J50" s="46" t="s">
-        <v>144</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J50" s="46"/>
       <c r="K50" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L50" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="50" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="N50" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O50" s="31"/>
     </row>
-    <row r="51" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
+    <row r="51" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A51" s="29" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>84</v>
+        <v>255</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>85</v>
+        <v>256</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>139</v>
+        <v>257</v>
       </c>
       <c r="F51" s="58"/>
       <c r="G51" s="58"/>
@@ -6039,28 +6043,26 @@
         <v>42843</v>
       </c>
       <c r="I51" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="J51" s="46" t="s">
-        <v>141</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J51" s="46"/>
       <c r="K51" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L51" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M51" s="50" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="N51" s="50" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="1:15" s="3" customFormat="1" ht="12.75">
       <c r="A52" s="59" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B52" s="60"/>
       <c r="C52" s="60"/>
@@ -6079,19 +6081,19 @@
     </row>
     <row r="53" spans="1:15" s="30" customFormat="1" ht="178.5" outlineLevel="1">
       <c r="A53" s="29" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E53" s="57" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F53" s="58"/>
       <c r="G53" s="58"/>
@@ -6103,34 +6105,34 @@
       </c>
       <c r="J53" s="37"/>
       <c r="K53" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L53" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M53" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N53" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O53" s="31"/>
     </row>
     <row r="54" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A54" s="29" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E54" s="57" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F54" s="58"/>
       <c r="G54" s="58"/>
@@ -6141,37 +6143,37 @@
         <v>0</v>
       </c>
       <c r="J54" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="K54" s="54" t="s">
         <v>143</v>
-      </c>
-      <c r="K54" s="54" t="s">
-        <v>154</v>
       </c>
       <c r="L54" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M54" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N54" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O54" s="31"/>
     </row>
     <row r="55" spans="1:15" s="30" customFormat="1" ht="165.75" outlineLevel="1">
       <c r="A55" s="29" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="E55" s="57" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F55" s="58"/>
       <c r="G55" s="58"/>
@@ -6183,34 +6185,34 @@
       </c>
       <c r="J55" s="37"/>
       <c r="K55" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L55" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M55" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N55" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O55" s="31"/>
     </row>
     <row r="56" spans="1:15" s="30" customFormat="1" ht="127.5" outlineLevel="1">
       <c r="A56" s="29" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E56" s="57" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F56" s="58"/>
       <c r="G56" s="58"/>
@@ -6221,37 +6223,37 @@
         <v>0</v>
       </c>
       <c r="J56" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="K56" s="54" t="s">
         <v>143</v>
-      </c>
-      <c r="K56" s="54" t="s">
-        <v>154</v>
       </c>
       <c r="L56" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M56" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N56" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O56" s="31"/>
     </row>
     <row r="57" spans="1:15" s="30" customFormat="1" ht="114.75" outlineLevel="1">
       <c r="A57" s="29" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E57" s="57" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="F57" s="58"/>
       <c r="G57" s="58"/>
@@ -6262,37 +6264,37 @@
         <v>0</v>
       </c>
       <c r="J57" s="46" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="K57" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L57" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M57" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N57" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O57" s="31"/>
     </row>
     <row r="58" spans="1:15" s="30" customFormat="1" ht="89.25" outlineLevel="1">
       <c r="A58" s="29" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E58" s="57" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F58" s="58"/>
       <c r="G58" s="58"/>
@@ -6303,37 +6305,37 @@
         <v>0</v>
       </c>
       <c r="J58" s="46" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="K58" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L58" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M58" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N58" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O58" s="31"/>
     </row>
     <row r="59" spans="1:15" s="30" customFormat="1" ht="153" outlineLevel="1">
       <c r="A59" s="29" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E59" s="57" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F59" s="58"/>
       <c r="G59" s="58"/>
@@ -6345,22 +6347,22 @@
       </c>
       <c r="J59" s="37"/>
       <c r="K59" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L59" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M59" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N59" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O59" s="31"/>
     </row>
     <row r="60" spans="1:15" s="3" customFormat="1" ht="12.75">
       <c r="A60" s="59" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B60" s="60"/>
       <c r="C60" s="60"/>
@@ -6379,19 +6381,19 @@
     </row>
     <row r="61" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A61" s="29" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E61" s="57" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F61" s="58"/>
       <c r="G61" s="58"/>
@@ -6403,34 +6405,34 @@
       </c>
       <c r="J61" s="46"/>
       <c r="K61" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L61" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M61" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N61" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O61" s="31"/>
     </row>
     <row r="62" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A62" s="29" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E62" s="57" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F62" s="58"/>
       <c r="G62" s="58"/>
@@ -6441,37 +6443,37 @@
         <v>0</v>
       </c>
       <c r="J62" s="46" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="K62" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L62" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M62" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N62" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O62" s="31"/>
     </row>
     <row r="63" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A63" s="29" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E63" s="57" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F63" s="58"/>
       <c r="G63" s="58"/>
@@ -6483,22 +6485,22 @@
       </c>
       <c r="J63" s="46"/>
       <c r="K63" s="54" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L63" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M63" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N63" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O63" s="31"/>
     </row>
     <row r="64" spans="1:15" s="3" customFormat="1" ht="12.75">
       <c r="A64" s="59" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B64" s="60"/>
       <c r="C64" s="60"/>
@@ -6517,19 +6519,19 @@
     </row>
     <row r="65" spans="1:15" s="30" customFormat="1" ht="25.5" outlineLevel="1">
       <c r="A65" s="29" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E65" s="57" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F65" s="58"/>
       <c r="G65" s="58"/>
@@ -6541,34 +6543,34 @@
       </c>
       <c r="J65" s="46"/>
       <c r="K65" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L65" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M65" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N65" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O65" s="31"/>
     </row>
     <row r="66" spans="1:15" s="30" customFormat="1" ht="63.75" outlineLevel="1">
       <c r="A66" s="29" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E66" s="57" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F66" s="58"/>
       <c r="G66" s="58"/>
@@ -6580,34 +6582,34 @@
       </c>
       <c r="J66" s="46"/>
       <c r="K66" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L66" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M66" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N66" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O66" s="31"/>
     </row>
     <row r="67" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A67" s="29" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E67" s="57" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F67" s="58"/>
       <c r="G67" s="58"/>
@@ -6619,34 +6621,34 @@
       </c>
       <c r="J67" s="46"/>
       <c r="K67" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L67" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M67" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N67" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O67" s="31"/>
     </row>
     <row r="68" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A68" s="29" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D68" s="28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E68" s="57" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F68" s="58"/>
       <c r="G68" s="58"/>
@@ -6657,37 +6659,37 @@
         <v>0</v>
       </c>
       <c r="J68" s="46" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="K68" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L68" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M68" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N68" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O68" s="31"/>
     </row>
     <row r="69" spans="1:15" s="30" customFormat="1" ht="76.5" outlineLevel="1">
       <c r="A69" s="29" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E69" s="57" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F69" s="58"/>
       <c r="G69" s="58"/>
@@ -6699,16 +6701,16 @@
       </c>
       <c r="J69" s="46"/>
       <c r="K69" s="54" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L69" s="28" t="s">
         <v>18</v>
       </c>
       <c r="M69" s="50" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N69" s="50" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="O69" s="31"/>
     </row>
@@ -11205,17 +11207,17 @@
       <formula>NOT(ISERROR(SEARCH("Automated",M60)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M65:M69 M38:M43 M13:M16 M18:M36 M45:M51 M61:M63 M53:M59">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M65:M69 M38:M43 M13:M16 M18:M36 M61:M63 M53:M59 M45:M51">
       <formula1>$S$1:$S$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N45:N51 N65:N69 N61:N63 N53:N59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13 N13:N16 N18:N36 N38:N43 N65:N69 N61:N63 N53:N59 N45:N51">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I45:I51 I65:I69 I61:I63 I54:I59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16 I18:I36 I38:I43 I65:I69 I61:I63 I54:I59 I45:I51">
       <formula1>$R$1:$R$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K45:K51 K65:K69 K61:K63 K53:K59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K16 K18:K36 K38:K43 K65:K69 K61:K63 K53:K59 K45:K51">
       <formula1>$Q$1:$Q$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>